<commit_message>
Latest push with updates
</commit_message>
<xml_diff>
--- a/Old_Gang_beck_raw_data_2025.xlsx
+++ b/Old_Gang_beck_raw_data_2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rgd531/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\SynologyDrive\Documents\University of York\BSc (Hons) Environmental Geography\3rd Year (2024-2025)\Pollution - Monitoring Assessment and Control\Assessment - Technical Report\Code and Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02684B69-EFE9-964E-845C-4DCF610A19B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC96BF5F-51C0-40AD-902E-1F53F0C25751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="940" windowWidth="25600" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Old Gang Beck Raw Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
   <si>
     <t>Label</t>
   </si>
@@ -167,9 +167,6 @@
     <t>SPENCE level repeat</t>
   </si>
   <si>
-    <t>Trib 3 USSPENCE Lv DS repeat</t>
-  </si>
-  <si>
     <t>Trib 3 repeat</t>
   </si>
   <si>
@@ -221,47 +218,6 @@
     <t>0.00153758863917055+H27:AC34</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve"> (us cm</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>mg l</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-  </si>
-  <si>
     <t>54.38187, -1.97616</t>
   </si>
   <si>
@@ -314,6 +270,9 @@
   </si>
   <si>
     <t>54.40116, -2.04433</t>
+  </si>
+  <si>
+    <t>Trib 3 US/SPENCE Lv DS repeat</t>
   </si>
 </sst>
 </file>
@@ -321,9 +280,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -457,13 +416,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <vertAlign val="superscript"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri (Body)"/>
     </font>
     <font>
       <sz val="18"/>
@@ -825,13 +777,13 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -888,10 +840,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1191,52 +1139,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC45"/>
+  <dimension ref="A1:AC44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.83203125" customWidth="1"/>
-    <col min="2" max="2" width="40.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="12" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="5" customFormat="1">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="C1" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>13</v>
@@ -1308,2140 +1262,2143 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="6" customFormat="1" ht="17">
-      <c r="A2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC2" s="6" t="s">
-        <v>63</v>
+    <row r="2" spans="1:29">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3.96</v>
+      </c>
+      <c r="D2">
+        <v>53</v>
+      </c>
+      <c r="E2" s="2">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3">
+        <v>2.56</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.30651736861052387</v>
+      </c>
+      <c r="H2" s="1">
+        <v>-1.4484563273877175E-3</v>
+      </c>
+      <c r="I2" s="1">
+        <v>5.9351431527796726E-2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>7.0819563409063799E-2</v>
+      </c>
+      <c r="K2" s="1">
+        <v>-3.023287254703915E-3</v>
+      </c>
+      <c r="L2" s="1">
+        <v>6.4525381630827576E-5</v>
+      </c>
+      <c r="M2" s="1">
+        <v>8.1485036142006856E-4</v>
+      </c>
+      <c r="N2" s="1">
+        <v>-1.5399594737112443E-2</v>
+      </c>
+      <c r="O2" s="1">
+        <v>2.6628156302901094E-3</v>
+      </c>
+      <c r="P2" s="1">
+        <v>5.1219693729126457E-2</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0.6231321824492827</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0.30383917276009353</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1.8076420499067815E-3</v>
+      </c>
+      <c r="T2" s="1">
+        <v>4.4401393244951175E-3</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0.84771388350360433</v>
+      </c>
+      <c r="V2" s="1">
+        <v>2.0802179980811343E-3</v>
+      </c>
+      <c r="W2" s="1">
+        <v>-2.1757889228477172E-3</v>
+      </c>
+      <c r="X2" s="1">
+        <v>4.3866379615259708E-4</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1.0131756977124595E-2</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>0.13998197757735242</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>2.397259288667076</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>7.3599602970493485E-4</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>0.28176020278247887</v>
       </c>
     </row>
     <row r="3" spans="1:29">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="3">
-        <v>3.96</v>
-      </c>
-      <c r="D3">
-        <v>53</v>
-      </c>
-      <c r="E3" s="2">
-        <v>12</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="E3" s="2"/>
       <c r="F3" s="3">
-        <v>2.56</v>
+        <v>3.51</v>
       </c>
       <c r="G3" s="1">
-        <v>0.30651736861052387</v>
+        <v>0.31515657120427004</v>
       </c>
       <c r="H3" s="1">
-        <v>-1.4484563273877175E-3</v>
+        <v>2.076270178692565E-4</v>
       </c>
       <c r="I3" s="1">
-        <v>5.9351431527796726E-2</v>
+        <v>5.9191109662670001E-2</v>
       </c>
       <c r="J3" s="1">
-        <v>7.0819563409063799E-2</v>
+        <v>6.9974184757377419E-2</v>
       </c>
       <c r="K3" s="1">
-        <v>-3.023287254703915E-3</v>
+        <v>-1.6382833971963738E-3</v>
       </c>
       <c r="L3" s="1">
-        <v>6.4525381630827576E-5</v>
+        <v>2.369785704484983E-4</v>
       </c>
       <c r="M3" s="1">
-        <v>8.1485036142006856E-4</v>
+        <v>1.1137221569924916E-3</v>
       </c>
       <c r="N3" s="1">
-        <v>-1.5399594737112443E-2</v>
+        <v>-1.6054310510951471E-2</v>
       </c>
       <c r="O3" s="1">
-        <v>2.6628156302901094E-3</v>
+        <v>1.4684596345009909E-3</v>
       </c>
       <c r="P3" s="1">
-        <v>5.1219693729126457E-2</v>
+        <v>5.0657848701157575E-2</v>
       </c>
       <c r="Q3" s="1">
-        <v>0.6231321824492827</v>
+        <v>0.61730966431754319</v>
       </c>
       <c r="R3" s="1">
-        <v>0.30383917276009353</v>
+        <v>0.30590135790501671</v>
       </c>
       <c r="S3" s="1">
-        <v>1.8076420499067815E-3</v>
+        <v>1.6908137322517367E-3</v>
       </c>
       <c r="T3" s="1">
-        <v>4.4401393244951175E-3</v>
+        <v>2.2495926529150297E-3</v>
       </c>
       <c r="U3" s="1">
-        <v>0.84771388350360433</v>
+        <v>0.85883348192205011</v>
       </c>
       <c r="V3" s="1">
-        <v>2.0802179980811343E-3</v>
+        <v>1.964908823003431E-3</v>
       </c>
       <c r="W3" s="1">
-        <v>-2.1757889228477172E-3</v>
+        <v>-1.9530937907785214E-3</v>
       </c>
       <c r="X3" s="1">
-        <v>4.3866379615259708E-4</v>
+        <v>7.6976669793307612E-5</v>
       </c>
       <c r="Y3" s="1">
-        <v>1.0131756977124595E-2</v>
+        <v>1.0065462948027933E-2</v>
       </c>
       <c r="Z3" s="1">
-        <v>0.13998197757735242</v>
+        <v>0.13983840683241003</v>
       </c>
       <c r="AA3" s="1">
-        <v>2.397259288667076</v>
+        <v>2.4311182660858965</v>
       </c>
       <c r="AB3" s="1">
-        <v>7.3599602970493485E-4</v>
+        <v>7.2505894667672073E-4</v>
       </c>
       <c r="AC3" s="1">
-        <v>0.28176020278247887</v>
+        <v>0.28538641799425118</v>
       </c>
     </row>
     <row r="4" spans="1:29">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="E4" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="C4" s="3">
+        <v>4.58</v>
+      </c>
+      <c r="D4">
+        <v>39</v>
+      </c>
+      <c r="E4" s="2">
+        <v>12</v>
+      </c>
       <c r="F4" s="3">
-        <v>3.51</v>
+        <v>11.1</v>
       </c>
       <c r="G4" s="1">
-        <v>0.31515657120427004</v>
+        <v>0.6372457860677857</v>
       </c>
       <c r="H4" s="1">
-        <v>2.076270178692565E-4</v>
+        <v>-1.0760253484809455E-3</v>
       </c>
       <c r="I4" s="1">
-        <v>5.9191109662670001E-2</v>
+        <v>0.29392382666082378</v>
       </c>
       <c r="J4" s="1">
-        <v>6.9974184757377419E-2</v>
+        <v>1.0548993458228064</v>
       </c>
       <c r="K4" s="1">
-        <v>-1.6382833971963738E-3</v>
+        <v>-2.4779745771697798E-3</v>
       </c>
       <c r="L4" s="1">
-        <v>2.369785704484983E-4</v>
+        <v>1.5389030696615427E-3</v>
       </c>
       <c r="M4" s="1">
-        <v>1.1137221569924916E-3</v>
+        <v>2.2045754409944227E-3</v>
       </c>
       <c r="N4" s="1">
-        <v>-1.6054310510951471E-2</v>
+        <v>-1.6119463182801327E-2</v>
       </c>
       <c r="O4" s="1">
-        <v>1.4684596345009909E-3</v>
+        <v>4.1432753822562042E-3</v>
       </c>
       <c r="P4" s="1">
-        <v>5.0657848701157575E-2</v>
+        <v>7.211846672963905E-2</v>
       </c>
       <c r="Q4" s="1">
-        <v>0.61730966431754319</v>
+        <v>0.63728593334838779</v>
       </c>
       <c r="R4" s="1">
-        <v>0.30590135790501671</v>
+        <v>0.39358499000404928</v>
       </c>
       <c r="S4" s="1">
-        <v>1.6908137322517367E-3</v>
+        <v>3.7072512103593597E-3</v>
       </c>
       <c r="T4" s="1">
-        <v>2.2495926529150297E-3</v>
+        <v>2.5899542593751592E-3</v>
       </c>
       <c r="U4" s="1">
-        <v>0.85883348192205011</v>
+        <v>3.4375326532649311</v>
       </c>
       <c r="V4" s="1">
-        <v>1.964908823003431E-3</v>
+        <v>5.6664143955374828E-3</v>
       </c>
       <c r="W4" s="1">
-        <v>-1.9530937907785214E-3</v>
+        <v>1.4116821240930924E-3</v>
       </c>
       <c r="X4" s="1">
-        <v>7.6976669793307612E-5</v>
+        <v>3.7300580435382344E-4</v>
       </c>
       <c r="Y4" s="1">
-        <v>1.0065462948027933E-2</v>
+        <v>6.6715992468928897E-2</v>
       </c>
       <c r="Z4" s="1">
-        <v>0.13983840683241003</v>
+        <v>0.73693938234950684</v>
       </c>
       <c r="AA4" s="1">
-        <v>2.4311182660858965</v>
+        <v>2.4487818328978728</v>
       </c>
       <c r="AB4" s="1">
-        <v>7.2505894667672073E-4</v>
+        <v>1.1111347224848174E-3</v>
       </c>
       <c r="AC4" s="1">
-        <v>0.28538641799425118</v>
+        <v>0.19967451165132419</v>
       </c>
     </row>
     <row r="5" spans="1:29">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="3">
-        <v>4.58</v>
-      </c>
-      <c r="D5">
-        <v>39</v>
-      </c>
-      <c r="E5" s="2">
-        <v>12</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="E5" s="2"/>
       <c r="F5" s="3">
-        <v>11.1</v>
+        <v>10.119999999999999</v>
       </c>
       <c r="G5" s="1">
-        <v>0.6372457860677857</v>
+        <v>0.64220240039412879</v>
       </c>
       <c r="H5" s="1">
-        <v>-1.0760253484809455E-3</v>
+        <v>-1.6316116965653619E-3</v>
       </c>
       <c r="I5" s="1">
-        <v>0.29392382666082378</v>
+        <v>0.29259620698678795</v>
       </c>
       <c r="J5" s="1">
-        <v>1.0548993458228064</v>
+        <v>1.0520323196135297</v>
       </c>
       <c r="K5" s="1">
-        <v>-2.4779745771697798E-3</v>
+        <v>-2.4662860417566413E-4</v>
       </c>
       <c r="L5" s="1">
-        <v>1.5389030696615427E-3</v>
+        <v>1.4222893214985387E-3</v>
       </c>
       <c r="M5" s="1">
-        <v>2.2045754409944227E-3</v>
+        <v>2.1776551547816928E-3</v>
       </c>
       <c r="N5" s="1">
-        <v>-1.6119463182801327E-2</v>
+        <v>-1.5857298128386241E-2</v>
       </c>
       <c r="O5" s="1">
-        <v>4.1432753822562042E-3</v>
+        <v>2.545142985165305E-3</v>
       </c>
       <c r="P5" s="1">
-        <v>7.211846672963905E-2</v>
+        <v>7.140339085696816E-2</v>
       </c>
       <c r="Q5" s="1">
-        <v>0.63728593334838779</v>
+        <v>0.63274808379827407</v>
       </c>
       <c r="R5" s="1">
-        <v>0.39358499000404928</v>
+        <v>0.39265875246626375</v>
       </c>
       <c r="S5" s="1">
-        <v>3.7072512103593597E-3</v>
+        <v>3.8521934484915649E-3</v>
       </c>
       <c r="T5" s="1">
-        <v>2.5899542593751592E-3</v>
+        <v>9.3653933450858968E-4</v>
       </c>
       <c r="U5" s="1">
-        <v>3.4375326532649311</v>
+        <v>3.4267081068183267</v>
       </c>
       <c r="V5" s="1">
-        <v>5.6664143955374828E-3</v>
+        <v>5.6566891350413526E-3</v>
       </c>
       <c r="W5" s="1">
-        <v>1.4116821240930924E-3</v>
+        <v>1.1231344638484555E-3</v>
       </c>
       <c r="X5" s="1">
-        <v>3.7300580435382344E-4</v>
+        <v>5.3226283267204008E-4</v>
       </c>
       <c r="Y5" s="1">
-        <v>6.6715992468928897E-2</v>
+        <v>6.6299594793662445E-2</v>
       </c>
       <c r="Z5" s="1">
-        <v>0.73693938234950684</v>
+        <v>0.73655172485893061</v>
       </c>
       <c r="AA5" s="1">
-        <v>2.4487818328978728</v>
+        <v>2.4544208699252406</v>
       </c>
       <c r="AB5" s="1">
-        <v>1.1111347224848174E-3</v>
+        <v>1.0379847377532936E-3</v>
       </c>
       <c r="AC5" s="1">
-        <v>0.19967451165132419</v>
+        <v>0.18789537847894502</v>
       </c>
     </row>
     <row r="6" spans="1:29">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="E6" s="2"/>
+        <v>73</v>
+      </c>
+      <c r="C6" s="3">
+        <v>6.8</v>
+      </c>
+      <c r="D6">
+        <v>52</v>
+      </c>
+      <c r="E6" s="2">
+        <v>12</v>
+      </c>
       <c r="F6" s="3">
-        <v>10.119999999999999</v>
+        <v>16.41</v>
       </c>
       <c r="G6" s="1">
-        <v>0.64220240039412879</v>
+        <v>0.28456454107885382</v>
       </c>
       <c r="H6" s="1">
-        <v>-1.6316116965653619E-3</v>
+        <v>-1.738623796597597E-3</v>
       </c>
       <c r="I6" s="1">
-        <v>0.29259620698678795</v>
+        <v>8.8885819167869792E-2</v>
       </c>
       <c r="J6" s="1">
-        <v>1.0520323196135297</v>
+        <v>5.6141154186094722E-2</v>
       </c>
       <c r="K6" s="1">
-        <v>-2.4662860417566413E-4</v>
+        <v>-1.753968315657696E-3</v>
       </c>
       <c r="L6" s="1">
-        <v>1.4222893214985387E-3</v>
+        <v>4.8378062770500463E-4</v>
       </c>
       <c r="M6" s="1">
-        <v>2.1776551547816928E-3</v>
+        <v>2.1684285609839785E-3</v>
       </c>
       <c r="N6" s="1">
-        <v>-1.5857298128386241E-2</v>
+        <v>-7.8694584993217343E-3</v>
       </c>
       <c r="O6" s="1">
-        <v>2.545142985165305E-3</v>
+        <v>6.6785850819345996E-3</v>
       </c>
       <c r="P6" s="1">
-        <v>7.140339085696816E-2</v>
+        <v>4.8661358369784802E-2</v>
       </c>
       <c r="Q6" s="1">
-        <v>0.63274808379827407</v>
+        <v>0.32273977262429171</v>
       </c>
       <c r="R6" s="1">
-        <v>0.39265875246626375</v>
+        <v>0.48301704723813071</v>
       </c>
       <c r="S6" s="1">
-        <v>3.8521934484915649E-3</v>
+        <v>1.367124942850056E-3</v>
       </c>
       <c r="T6" s="1">
-        <v>9.3653933450858968E-4</v>
+        <v>3.8159046952288334E-3</v>
       </c>
       <c r="U6" s="1">
-        <v>3.4267081068183267</v>
+        <v>5.812051522351612</v>
       </c>
       <c r="V6" s="1">
-        <v>5.6566891350413526E-3</v>
+        <v>1.5380830428985148E-3</v>
       </c>
       <c r="W6" s="1">
-        <v>1.1231344638484555E-3</v>
+        <v>2.7403660317428503E-3</v>
       </c>
       <c r="X6" s="1">
-        <v>5.3226283267204008E-4</v>
+        <v>5.1941556603652208E-4</v>
       </c>
       <c r="Y6" s="1">
-        <v>6.6299594793662445E-2</v>
+        <v>3.4899452170937761E-2</v>
       </c>
       <c r="Z6" s="1">
-        <v>0.73655172485893061</v>
+        <v>0.2328865375559547</v>
       </c>
       <c r="AA6" s="1">
-        <v>2.4544208699252406</v>
+        <v>2.7201182381276019</v>
       </c>
       <c r="AB6" s="1">
-        <v>1.0379847377532936E-3</v>
+        <v>8.6376727594609647E-4</v>
       </c>
       <c r="AC6" s="1">
-        <v>0.18789537847894502</v>
+        <v>0.20039546029230079</v>
       </c>
     </row>
     <row r="7" spans="1:29">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7" s="3">
-        <v>6.8</v>
-      </c>
-      <c r="D7">
-        <v>52</v>
-      </c>
-      <c r="E7" s="2">
-        <v>12</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="E7" s="2"/>
       <c r="F7" s="3">
-        <v>16.41</v>
+        <v>16.34</v>
       </c>
       <c r="G7" s="1">
-        <v>0.28456454107885382</v>
+        <v>0.28904594157007896</v>
       </c>
       <c r="H7" s="1">
-        <v>-1.738623796597597E-3</v>
+        <v>-1.1507750083513968E-3</v>
       </c>
       <c r="I7" s="1">
-        <v>8.8885819167869792E-2</v>
+        <v>8.9191954299904605E-2</v>
       </c>
       <c r="J7" s="1">
-        <v>5.6141154186094722E-2</v>
+        <v>5.5667285310767263E-2</v>
       </c>
       <c r="K7" s="1">
-        <v>-1.753968315657696E-3</v>
+        <v>1.7085914023693201E-3</v>
       </c>
       <c r="L7" s="1">
-        <v>4.8378062770500463E-4</v>
+        <v>3.392133019256545E-4</v>
       </c>
       <c r="M7" s="1">
-        <v>2.1684285609839785E-3</v>
+        <v>1.6320166555204272E-3</v>
       </c>
       <c r="N7" s="1">
-        <v>-7.8694584993217343E-3</v>
+        <v>-7.8570788886212738E-3</v>
       </c>
       <c r="O7" s="1">
-        <v>6.6785850819345996E-3</v>
+        <v>3.3977148410836273E-3</v>
       </c>
       <c r="P7" s="1">
-        <v>4.8661358369784802E-2</v>
+        <v>4.8037171159520754E-2</v>
       </c>
       <c r="Q7" s="1">
-        <v>0.32273977262429171</v>
+        <v>0.32324616923776323</v>
       </c>
       <c r="R7" s="1">
-        <v>0.48301704723813071</v>
+        <v>0.48091182153994394</v>
       </c>
       <c r="S7" s="1">
-        <v>1.367124942850056E-3</v>
+        <v>1.1233874530399881E-3</v>
       </c>
       <c r="T7" s="1">
-        <v>3.8159046952288334E-3</v>
+        <v>5.0731629331517694E-3</v>
       </c>
       <c r="U7" s="1">
-        <v>5.812051522351612</v>
+        <v>5.8165589000751021</v>
       </c>
       <c r="V7" s="1">
-        <v>1.5380830428985148E-3</v>
+        <v>1.6390604691140975E-3</v>
       </c>
       <c r="W7" s="1">
-        <v>2.7403660317428503E-3</v>
+        <v>-2.3145536901805113E-4</v>
       </c>
       <c r="X7" s="1">
-        <v>5.1941556603652208E-4</v>
+        <v>5.9618561479112128E-4</v>
       </c>
       <c r="Y7" s="1">
-        <v>3.4899452170937761E-2</v>
+        <v>3.4820007416102611E-2</v>
       </c>
       <c r="Z7" s="1">
-        <v>0.2328865375559547</v>
+        <v>0.23336123914248078</v>
       </c>
       <c r="AA7" s="1">
-        <v>2.7201182381276019</v>
+        <v>2.7481706791287337</v>
       </c>
       <c r="AB7" s="1">
-        <v>8.6376727594609647E-4</v>
+        <v>8.0308416634390471E-4</v>
       </c>
       <c r="AC7" s="1">
-        <v>0.20039546029230079</v>
+        <v>0.19217604037209327</v>
       </c>
     </row>
     <row r="8" spans="1:29">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="E8" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C8" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="D8">
+        <v>42</v>
+      </c>
+      <c r="E8" s="2">
+        <v>12</v>
+      </c>
       <c r="F8" s="3">
-        <v>16.34</v>
+        <v>11.17</v>
       </c>
       <c r="G8" s="1">
-        <v>0.28904594157007896</v>
+        <v>0.48527666717832924</v>
       </c>
       <c r="H8" s="1">
-        <v>-1.1507750083513968E-3</v>
+        <v>-9.0883879212143683E-4</v>
       </c>
       <c r="I8" s="1">
-        <v>8.9191954299904605E-2</v>
+        <v>0.20129112936991644</v>
       </c>
       <c r="J8" s="1">
-        <v>5.5667285310767263E-2</v>
+        <v>0.36355136372065289</v>
       </c>
       <c r="K8" s="1">
-        <v>1.7085914023693201E-3</v>
+        <v>-1.5784088257179512E-3</v>
       </c>
       <c r="L8" s="1">
-        <v>3.392133019256545E-4</v>
+        <v>1.1550606202994052E-3</v>
       </c>
       <c r="M8" s="1">
-        <v>1.6320166555204272E-3</v>
+        <v>2.1361315463491234E-3</v>
       </c>
       <c r="N8" s="1">
-        <v>-7.8570788886212738E-3</v>
+        <v>-1.1446987434949665E-2</v>
       </c>
       <c r="O8" s="1">
-        <v>3.3977148410836273E-3</v>
+        <v>4.8240998995292455E-3</v>
       </c>
       <c r="P8" s="1">
-        <v>4.8037171159520754E-2</v>
+        <v>5.3115524565906715E-2</v>
       </c>
       <c r="Q8" s="1">
-        <v>0.32324616923776323</v>
+        <v>0.46834082705214564</v>
       </c>
       <c r="R8" s="1">
-        <v>0.48091182153994394</v>
+        <v>0.41395035816075382</v>
       </c>
       <c r="S8" s="1">
-        <v>1.1233874530399881E-3</v>
+        <v>1.699952239127096E-3</v>
       </c>
       <c r="T8" s="1">
-        <v>5.0731629331517694E-3</v>
+        <v>1.876903056041903E-3</v>
       </c>
       <c r="U8" s="1">
-        <v>5.8165589000751021</v>
+        <v>3.7815233663452923</v>
       </c>
       <c r="V8" s="1">
-        <v>1.6390604691140975E-3</v>
+        <v>4.6853890901647254E-3</v>
       </c>
       <c r="W8" s="1">
-        <v>-2.3145536901805113E-4</v>
+        <v>-6.4104936679179516E-4</v>
       </c>
       <c r="X8" s="1">
-        <v>5.9618561479112128E-4</v>
+        <v>1.769328214366447E-4</v>
       </c>
       <c r="Y8" s="1">
-        <v>3.4820007416102611E-2</v>
+        <v>5.172046580253184E-2</v>
       </c>
       <c r="Z8" s="1">
-        <v>0.23336123914248078</v>
+        <v>0.47598861629228378</v>
       </c>
       <c r="AA8" s="1">
-        <v>2.7481706791287337</v>
+        <v>2.5312299753068328</v>
       </c>
       <c r="AB8" s="1">
-        <v>8.0308416634390471E-4</v>
+        <v>1.0552762880230832E-3</v>
       </c>
       <c r="AC8" s="1">
-        <v>0.19217604037209327</v>
+        <v>0.22061290447159718</v>
       </c>
     </row>
     <row r="9" spans="1:29">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="D9">
-        <v>42</v>
-      </c>
-      <c r="E9" s="2">
-        <v>12</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="E9" s="2"/>
       <c r="F9" s="3">
-        <v>11.17</v>
+        <v>11.46</v>
       </c>
       <c r="G9" s="1">
-        <v>0.48527666717832924</v>
+        <v>0.49774871176541308</v>
       </c>
       <c r="H9" s="1">
-        <v>-9.0883879212143683E-4</v>
+        <v>-1.4539497675797267E-3</v>
       </c>
       <c r="I9" s="1">
-        <v>0.20129112936991644</v>
+        <v>0.20033045476902736</v>
       </c>
       <c r="J9" s="1">
-        <v>0.36355136372065289</v>
+        <v>0.36220029363503031</v>
       </c>
       <c r="K9" s="1">
-        <v>-1.5784088257179512E-3</v>
+        <v>1.8326525696701094E-3</v>
       </c>
       <c r="L9" s="1">
-        <v>1.1550606202994052E-3</v>
+        <v>1.1927295832394828E-3</v>
       </c>
       <c r="M9" s="1">
-        <v>2.1361315463491234E-3</v>
+        <v>1.9301808606314377E-3</v>
       </c>
       <c r="N9" s="1">
-        <v>-1.1446987434949665E-2</v>
+        <v>-1.1105410135924096E-2</v>
       </c>
       <c r="O9" s="1">
-        <v>4.8240998995292455E-3</v>
+        <v>2.6499209415773357E-3</v>
       </c>
       <c r="P9" s="1">
-        <v>5.3115524565906715E-2</v>
+        <v>5.2703050787826056E-2</v>
       </c>
       <c r="Q9" s="1">
-        <v>0.46834082705214564</v>
+        <v>0.465160369984088</v>
       </c>
       <c r="R9" s="1">
-        <v>0.41395035816075382</v>
+        <v>0.41632128325582829</v>
       </c>
       <c r="S9" s="1">
-        <v>1.699952239127096E-3</v>
+        <v>1.5388651615400237E-3</v>
       </c>
       <c r="T9" s="1">
-        <v>1.876903056041903E-3</v>
+        <v>3.1681086085670169E-3</v>
       </c>
       <c r="U9" s="1">
-        <v>3.7815233663452923</v>
+        <v>3.8070665676721305</v>
       </c>
       <c r="V9" s="1">
-        <v>4.6853890901647254E-3</v>
+        <v>4.921037746454175E-3</v>
       </c>
       <c r="W9" s="1">
-        <v>-6.4104936679179516E-4</v>
+        <v>9.4403656860562752E-4</v>
       </c>
       <c r="X9" s="1">
-        <v>1.769328214366447E-4</v>
+        <v>8.4860401403827929E-6</v>
       </c>
       <c r="Y9" s="1">
-        <v>5.172046580253184E-2</v>
+        <v>5.1540364652524144E-2</v>
       </c>
       <c r="Z9" s="1">
-        <v>0.47598861629228378</v>
+        <v>0.47599899272364815</v>
       </c>
       <c r="AA9" s="1">
-        <v>2.5312299753068328</v>
+        <v>2.5649474845763511</v>
       </c>
       <c r="AB9" s="1">
-        <v>1.0552762880230832E-3</v>
+        <v>9.6095452779672557E-4</v>
       </c>
       <c r="AC9" s="1">
-        <v>0.22061290447159718</v>
+        <v>0.19513838294255323</v>
       </c>
     </row>
     <row r="10" spans="1:29">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="E10" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="C10" s="3">
+        <v>7.32</v>
+      </c>
+      <c r="D10">
+        <v>67</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
       <c r="F10" s="3">
-        <v>11.46</v>
+        <v>23.92</v>
       </c>
       <c r="G10" s="1">
-        <v>0.49774871176541308</v>
+        <v>0.28229961678203458</v>
       </c>
       <c r="H10" s="1">
-        <v>-1.4539497675797267E-3</v>
+        <v>-2.4214584778313175E-3</v>
       </c>
       <c r="I10" s="1">
-        <v>0.20033045476902736</v>
+        <v>0.15308140672644804</v>
       </c>
       <c r="J10" s="1">
-        <v>0.36220029363503031</v>
+        <v>0.23312438695912688</v>
       </c>
       <c r="K10" s="1">
-        <v>1.8326525696701094E-3</v>
+        <v>-7.2301019359067686E-4</v>
       </c>
       <c r="L10" s="1">
-        <v>1.1927295832394828E-3</v>
+        <v>8.3833898343750254E-4</v>
       </c>
       <c r="M10" s="1">
-        <v>1.9301808606314377E-3</v>
+        <v>1.6440227789864174E-3</v>
       </c>
       <c r="N10" s="1">
-        <v>-1.1105410135924096E-2</v>
+        <v>-1.0200060195403583E-2</v>
       </c>
       <c r="O10" s="1">
-        <v>2.6499209415773357E-3</v>
+        <v>1.9037203278151951E-3</v>
       </c>
       <c r="P10" s="1">
-        <v>5.2703050787826056E-2</v>
+        <v>3.2839121190236319E-2</v>
       </c>
       <c r="Q10" s="1">
-        <v>0.465160369984088</v>
+        <v>0.39538594342745742</v>
       </c>
       <c r="R10" s="1">
-        <v>0.41632128325582829</v>
+        <v>0.70591810821431389</v>
       </c>
       <c r="S10" s="1">
-        <v>1.5388651615400237E-3</v>
+        <v>1.3794441541607029E-3</v>
       </c>
       <c r="T10" s="1">
-        <v>3.1681086085670169E-3</v>
+        <v>1.0747123794394514E-3</v>
       </c>
       <c r="U10" s="1">
-        <v>3.8070665676721305</v>
+        <v>8.4159798750403425</v>
       </c>
       <c r="V10" s="1">
-        <v>4.921037746454175E-3</v>
+        <v>1.1219153500506292E-2</v>
       </c>
       <c r="W10" s="1">
-        <v>9.4403656860562752E-4</v>
+        <v>-3.6615376414665213E-3</v>
       </c>
       <c r="X10" s="1">
-        <v>8.4860401403827929E-6</v>
+        <v>-9.0648013947954652E-5</v>
       </c>
       <c r="Y10" s="1">
-        <v>5.1540364652524144E-2</v>
+        <v>9.7815184960823351E-2</v>
       </c>
       <c r="Z10" s="1">
-        <v>0.47599899272364815</v>
+        <v>0.45779686211588072</v>
       </c>
       <c r="AA10" s="1">
-        <v>2.5649474845763511</v>
+        <v>2.7849962145323652</v>
       </c>
       <c r="AB10" s="1">
-        <v>9.6095452779672557E-4</v>
+        <v>1.4511404731576284E-3</v>
       </c>
       <c r="AC10" s="1">
-        <v>0.19513838294255323</v>
+        <v>0.23248727207161382</v>
       </c>
     </row>
     <row r="11" spans="1:29">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" s="3">
-        <v>7.32</v>
-      </c>
-      <c r="D11">
-        <v>67</v>
-      </c>
-      <c r="E11" s="2">
-        <v>5</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="E11" s="2"/>
       <c r="F11" s="3">
-        <v>23.92</v>
+        <v>24.01</v>
       </c>
       <c r="G11" s="1">
-        <v>0.28229961678203458</v>
+        <v>0.27809982617350837</v>
       </c>
       <c r="H11" s="1">
-        <v>-2.4214584778313175E-3</v>
+        <v>-2.2746430092734061E-3</v>
       </c>
       <c r="I11" s="1">
-        <v>0.15308140672644804</v>
+        <v>0.15336079934861571</v>
       </c>
       <c r="J11" s="1">
-        <v>0.23312438695912688</v>
+        <v>0.23295816599524696</v>
       </c>
       <c r="K11" s="1">
-        <v>-7.2301019359067686E-4</v>
+        <v>-2.3616301390726284E-3</v>
       </c>
       <c r="L11" s="1">
-        <v>8.3833898343750254E-4</v>
+        <v>8.4067431039712393E-4</v>
       </c>
       <c r="M11" s="1">
-        <v>1.6440227789864174E-3</v>
+        <v>2.0743639483180695E-3</v>
       </c>
       <c r="N11" s="1">
-        <v>-1.0200060195403583E-2</v>
+        <v>-9.9499637471983388E-3</v>
       </c>
       <c r="O11" s="1">
-        <v>1.9037203278151951E-3</v>
+        <v>2.9224241308906467E-3</v>
       </c>
       <c r="P11" s="1">
-        <v>3.2839121190236319E-2</v>
+        <v>3.3106503608507455E-2</v>
       </c>
       <c r="Q11" s="1">
-        <v>0.39538594342745742</v>
+        <v>0.39795227154927293</v>
       </c>
       <c r="R11" s="1">
-        <v>0.70591810821431389</v>
+        <v>0.7093611440674561</v>
       </c>
       <c r="S11" s="1">
-        <v>1.3794441541607029E-3</v>
+        <v>1.5130579821241222E-3</v>
       </c>
       <c r="T11" s="1">
-        <v>1.0747123794394514E-3</v>
+        <v>2.6173538284161978E-3</v>
       </c>
       <c r="U11" s="1">
-        <v>8.4159798750403425</v>
+        <v>8.436851389537189</v>
       </c>
       <c r="V11" s="1">
-        <v>1.1219153500506292E-2</v>
+        <v>1.1063864911496551E-2</v>
       </c>
       <c r="W11" s="1">
-        <v>-3.6615376414665213E-3</v>
+        <v>5.2632880052460847E-4</v>
       </c>
       <c r="X11" s="1">
-        <v>-9.0648013947954652E-5</v>
+        <v>5.2584948302580663E-4</v>
       </c>
       <c r="Y11" s="1">
-        <v>9.7815184960823351E-2</v>
+        <v>9.8668123149362019E-2</v>
       </c>
       <c r="Z11" s="1">
-        <v>0.45779686211588072</v>
+        <v>0.45955827615505257</v>
       </c>
       <c r="AA11" s="1">
-        <v>2.7849962145323652</v>
+        <v>2.7666458618805088</v>
       </c>
       <c r="AB11" s="1">
-        <v>1.4511404731576284E-3</v>
+        <v>1.4770878240728178E-3</v>
       </c>
       <c r="AC11" s="1">
-        <v>0.23248727207161382</v>
+        <v>0.23466047135173049</v>
       </c>
     </row>
     <row r="12" spans="1:29">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="E12" s="2"/>
+        <v>70</v>
+      </c>
+      <c r="C12" s="3">
+        <v>7.81</v>
+      </c>
+      <c r="D12">
+        <v>212</v>
+      </c>
+      <c r="E12" s="2">
+        <v>25</v>
+      </c>
       <c r="F12" s="3">
-        <v>24.01</v>
+        <v>86.7</v>
       </c>
       <c r="G12" s="1">
-        <v>0.27809982617350837</v>
+        <v>0.12035692448986766</v>
       </c>
       <c r="H12" s="1">
-        <v>-2.2746430092734061E-3</v>
+        <v>-7.942231602463438E-4</v>
       </c>
       <c r="I12" s="1">
-        <v>0.15336079934861571</v>
+        <v>0.58932393897995083</v>
       </c>
       <c r="J12" s="1">
-        <v>0.23295816599524696</v>
+        <v>0.11228116276641538</v>
       </c>
       <c r="K12" s="1">
-        <v>-2.3616301390726284E-3</v>
+        <v>-2.1873636347906418E-3</v>
       </c>
       <c r="L12" s="1">
-        <v>8.4067431039712393E-4</v>
+        <v>4.5897847333114918E-3</v>
       </c>
       <c r="M12" s="1">
-        <v>2.0743639483180695E-3</v>
+        <v>2.8418463855911617E-3</v>
       </c>
       <c r="N12" s="1">
-        <v>-9.9499637471983388E-3</v>
+        <v>-2.1702085124030786E-3</v>
       </c>
       <c r="O12" s="1">
-        <v>2.9224241308906467E-3</v>
+        <v>7.1940215780911384E-3</v>
       </c>
       <c r="P12" s="1">
-        <v>3.3106503608507455E-2</v>
+        <v>4.4754802064707281E-3</v>
       </c>
       <c r="Q12" s="1">
-        <v>0.39795227154927293</v>
+        <v>8.4220995996329803E-2</v>
       </c>
       <c r="R12" s="1">
-        <v>0.7093611440674561</v>
+        <v>2.9325447367347031</v>
       </c>
       <c r="S12" s="1">
-        <v>1.5130579821241222E-3</v>
+        <v>9.5002528285280418E-4</v>
       </c>
       <c r="T12" s="1">
-        <v>2.6173538284161978E-3</v>
+        <v>1.5464659090155812E-3</v>
       </c>
       <c r="U12" s="1">
-        <v>8.436851389537189</v>
+        <v>29.862723381414472</v>
       </c>
       <c r="V12" s="1">
-        <v>1.1063864911496551E-2</v>
+        <v>3.196276034188456E-3</v>
       </c>
       <c r="W12" s="1">
-        <v>5.2632880052460847E-4</v>
+        <v>3.4186134210846992E-4</v>
       </c>
       <c r="X12" s="1">
-        <v>5.2584948302580663E-4</v>
+        <v>4.960403048155297E-4</v>
       </c>
       <c r="Y12" s="1">
-        <v>9.8668123149362019E-2</v>
+        <v>0.49164515200111203</v>
       </c>
       <c r="Z12" s="1">
-        <v>0.45955827615505257</v>
+        <v>0.37026978999818266</v>
       </c>
       <c r="AA12" s="1">
-        <v>2.7666458618805088</v>
+        <v>3.4028294037814484</v>
       </c>
       <c r="AB12" s="1">
-        <v>1.4770878240728178E-3</v>
+        <v>8.7163161081039702E-3</v>
       </c>
       <c r="AC12" s="1">
-        <v>0.23466047135173049</v>
+        <v>0.61337278395773343</v>
       </c>
     </row>
     <row r="13" spans="1:29">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="3">
-        <v>7.81</v>
-      </c>
-      <c r="D13">
-        <v>212</v>
-      </c>
-      <c r="E13" s="2">
-        <v>25</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="3">
-        <v>86.7</v>
+        <v>86.1</v>
       </c>
       <c r="G13" s="1">
-        <v>0.12035692448986766</v>
+        <v>0.12383762984576369</v>
       </c>
       <c r="H13" s="1">
-        <v>-7.942231602463438E-4</v>
+        <v>-3.1959601080415296E-3</v>
       </c>
       <c r="I13" s="1">
-        <v>0.58932393897995083</v>
+        <v>0.58753035880745674</v>
       </c>
       <c r="J13" s="1">
-        <v>0.11228116276641538</v>
+        <v>0.11181729771500164</v>
       </c>
       <c r="K13" s="1">
-        <v>-2.1873636347906418E-3</v>
+        <v>-6.9087637118936439E-4</v>
       </c>
       <c r="L13" s="1">
-        <v>4.5897847333114918E-3</v>
+        <v>4.6411113534784486E-3</v>
       </c>
       <c r="M13" s="1">
-        <v>2.8418463855911617E-3</v>
+        <v>2.9261688796167074E-3</v>
       </c>
       <c r="N13" s="1">
-        <v>-2.1702085124030786E-3</v>
+        <v>-1.9758121229740753E-3</v>
       </c>
       <c r="O13" s="1">
-        <v>7.1940215780911384E-3</v>
+        <v>5.8735393970868995E-3</v>
       </c>
       <c r="P13" s="1">
-        <v>4.4754802064707281E-3</v>
+        <v>4.4143665928929885E-3</v>
       </c>
       <c r="Q13" s="1">
-        <v>8.4220995996329803E-2</v>
+        <v>8.3516059627965933E-2</v>
       </c>
       <c r="R13" s="1">
-        <v>2.9325447367347031</v>
+        <v>2.9184185477337317</v>
       </c>
       <c r="S13" s="1">
-        <v>9.5002528285280418E-4</v>
+        <v>8.929661295605522E-4</v>
       </c>
       <c r="T13" s="1">
-        <v>1.5464659090155812E-3</v>
+        <v>1.0606957416672864E-3</v>
       </c>
       <c r="U13" s="1">
-        <v>29.862723381414472</v>
+        <v>29.645470341972125</v>
       </c>
       <c r="V13" s="1">
-        <v>3.196276034188456E-3</v>
+        <v>3.1877012120615795E-3</v>
       </c>
       <c r="W13" s="1">
-        <v>3.4186134210846992E-4</v>
+        <v>9.7186328333417633E-4</v>
       </c>
       <c r="X13" s="1">
-        <v>4.960403048155297E-4</v>
+        <v>4.1633101527455748E-4</v>
       </c>
       <c r="Y13" s="1">
-        <v>0.49164515200111203</v>
+        <v>0.48913082872387398</v>
       </c>
       <c r="Z13" s="1">
-        <v>0.37026978999818266</v>
+        <v>0.36833668353564519</v>
       </c>
       <c r="AA13" s="1">
-        <v>3.4028294037814484</v>
+        <v>3.3883694052953488</v>
       </c>
       <c r="AB13" s="1">
-        <v>8.7163161081039702E-3</v>
+        <v>8.5627250598454049E-3</v>
       </c>
       <c r="AC13" s="1">
-        <v>0.61337278395773343</v>
+        <v>0.61476146366394391</v>
       </c>
     </row>
     <row r="14" spans="1:29">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="E14" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="C14" s="3">
+        <v>7.9</v>
+      </c>
+      <c r="D14">
+        <v>111</v>
+      </c>
+      <c r="E14" s="2">
+        <v>10</v>
+      </c>
       <c r="F14" s="3">
-        <v>86.1</v>
+        <v>40.229999999999997</v>
       </c>
       <c r="G14" s="1">
-        <v>0.12383762984576369</v>
+        <v>0.11621579305441328</v>
       </c>
       <c r="H14" s="1">
-        <v>-3.1959601080415296E-3</v>
+        <v>-9.5396367187827562E-4</v>
       </c>
       <c r="I14" s="1">
-        <v>0.58753035880745674</v>
+        <v>0.20210061294712686</v>
       </c>
       <c r="J14" s="1">
-        <v>0.11181729771500164</v>
+        <v>4.902289603204904E-2</v>
       </c>
       <c r="K14" s="1">
-        <v>-6.9087637118936439E-4</v>
+        <v>1.9859978964807765E-4</v>
       </c>
       <c r="L14" s="1">
-        <v>4.6411113534784486E-3</v>
+        <v>3.4441436175708194E-4</v>
       </c>
       <c r="M14" s="1">
-        <v>2.9261688796167074E-3</v>
+        <v>1.5803110493725781E-3</v>
       </c>
       <c r="N14" s="1">
-        <v>-1.9758121229740753E-3</v>
+        <v>-2.5234072766808294E-3</v>
       </c>
       <c r="O14" s="1">
-        <v>5.8735393970868995E-3</v>
+        <v>4.6146770213231075E-3</v>
       </c>
       <c r="P14" s="1">
-        <v>4.4143665928929885E-3</v>
+        <v>9.6526953185132897E-3</v>
       </c>
       <c r="Q14" s="1">
-        <v>8.3516059627965933E-2</v>
+        <v>0.11435310488839705</v>
       </c>
       <c r="R14" s="1">
-        <v>2.9184185477337317</v>
+        <v>0.8507795485332319</v>
       </c>
       <c r="S14" s="1">
-        <v>8.929661295605522E-4</v>
+        <v>1.1266210918821696E-3</v>
       </c>
       <c r="T14" s="1">
-        <v>1.0606957416672864E-3</v>
+        <v>2.1632765314716163E-3</v>
       </c>
       <c r="U14" s="1">
-        <v>29.645470341972125</v>
+        <v>14.814768440944617</v>
       </c>
       <c r="V14" s="1">
-        <v>3.1877012120615795E-3</v>
+        <v>1.3190919138402178E-3</v>
       </c>
       <c r="W14" s="1">
-        <v>9.7186328333417633E-4</v>
+        <v>-2.4540754382689507E-3</v>
       </c>
       <c r="X14" s="1">
-        <v>4.1633101527455748E-4</v>
+        <v>1.8209172902175659E-4</v>
       </c>
       <c r="Y14" s="1">
-        <v>0.48913082872387398</v>
+        <v>6.8981151890739681E-2</v>
       </c>
       <c r="Z14" s="1">
-        <v>0.36833668353564519</v>
+        <v>0.18382964093734469</v>
       </c>
       <c r="AA14" s="1">
-        <v>3.3883694052953488</v>
+        <v>3.4210889937167646</v>
       </c>
       <c r="AB14" s="1">
-        <v>8.5627250598454049E-3</v>
+        <v>3.0960405106468525E-3</v>
       </c>
       <c r="AC14" s="1">
-        <v>0.61476146366394391</v>
+        <v>0.36045313152532032</v>
       </c>
     </row>
     <row r="15" spans="1:29">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="3">
-        <v>7.9</v>
-      </c>
-      <c r="D15">
-        <v>111</v>
-      </c>
-      <c r="E15" s="2">
-        <v>10</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="E15" s="2"/>
       <c r="F15" s="3">
-        <v>40.229999999999997</v>
+        <v>40.67</v>
       </c>
       <c r="G15" s="1">
-        <v>0.11621579305441328</v>
+        <v>0.11863216180890974</v>
       </c>
       <c r="H15" s="1">
-        <v>-9.5396367187827562E-4</v>
+        <v>-1.5599962372254434E-3</v>
       </c>
       <c r="I15" s="1">
-        <v>0.20210061294712686</v>
+        <v>0.20233444119113905</v>
       </c>
       <c r="J15" s="1">
-        <v>4.902289603204904E-2</v>
+        <v>4.8690808313638416E-2</v>
       </c>
       <c r="K15" s="1">
-        <v>1.9859978964807765E-4</v>
+        <v>3.8881859499051808E-5</v>
       </c>
       <c r="L15" s="1">
-        <v>3.4441436175708194E-4</v>
+        <v>4.7692845090864354E-4</v>
       </c>
       <c r="M15" s="1">
-        <v>1.5803110493725781E-3</v>
+        <v>1.5214132735586053E-3</v>
       </c>
       <c r="N15" s="1">
-        <v>-2.5234072766808294E-3</v>
+        <v>-2.8517345588757515E-3</v>
       </c>
       <c r="O15" s="1">
-        <v>4.6146770213231075E-3</v>
+        <v>2.8507013697577528E-3</v>
       </c>
       <c r="P15" s="1">
-        <v>9.6526953185132897E-3</v>
+        <v>9.5873362745419622E-3</v>
       </c>
       <c r="Q15" s="1">
-        <v>0.11435310488839705</v>
+        <v>0.11498449208889376</v>
       </c>
       <c r="R15" s="1">
-        <v>0.8507795485332319</v>
+        <v>0.85404709617325736</v>
       </c>
       <c r="S15" s="1">
-        <v>1.1266210918821696E-3</v>
+        <v>1.0528903902766939E-3</v>
       </c>
       <c r="T15" s="1">
-        <v>2.1632765314716163E-3</v>
+        <v>2.3517058844245756E-3</v>
       </c>
       <c r="U15" s="1">
-        <v>14.814768440944617</v>
+        <v>14.894373487473009</v>
       </c>
       <c r="V15" s="1">
-        <v>1.3190919138402178E-3</v>
+        <v>1.3620663984584868E-3</v>
       </c>
       <c r="W15" s="1">
-        <v>-2.4540754382689507E-3</v>
+        <v>-3.4691389208015656E-4</v>
       </c>
       <c r="X15" s="1">
-        <v>1.8209172902175659E-4</v>
+        <v>4.4828932653077225E-4</v>
       </c>
       <c r="Y15" s="1">
-        <v>6.8981151890739681E-2</v>
+        <v>6.8767064908112907E-2</v>
       </c>
       <c r="Z15" s="1">
-        <v>0.18382964093734469</v>
+        <v>0.18430166249340973</v>
       </c>
       <c r="AA15" s="1">
-        <v>3.4210889937167646</v>
+        <v>3.4691145174237725</v>
       </c>
       <c r="AB15" s="1">
-        <v>3.0960405106468525E-3</v>
+        <v>3.0340490881591692E-3</v>
       </c>
       <c r="AC15" s="1">
-        <v>0.36045313152532032</v>
+        <v>0.34453499239003743</v>
       </c>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="E16" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="C16" s="3">
+        <v>7.97</v>
+      </c>
+      <c r="D16">
+        <v>136</v>
+      </c>
+      <c r="E16" s="2">
+        <v>4</v>
+      </c>
       <c r="F16" s="3">
-        <v>40.67</v>
+        <v>51.43</v>
       </c>
       <c r="G16" s="1">
-        <v>0.11863216180890974</v>
+        <v>0.13030325861004863</v>
       </c>
       <c r="H16" s="1">
-        <v>-1.5599962372254434E-3</v>
+        <v>-1.9243036335420927E-3</v>
       </c>
       <c r="I16" s="1">
-        <v>0.20233444119113905</v>
+        <v>0.13984916284508361</v>
       </c>
       <c r="J16" s="1">
-        <v>4.8690808313638416E-2</v>
+        <v>9.9867131154848687E-2</v>
       </c>
       <c r="K16" s="1">
-        <v>3.8881859499051808E-5</v>
+        <v>-1.6014814303847198E-4</v>
       </c>
       <c r="L16" s="1">
-        <v>4.7692845090864354E-4</v>
+        <v>6.9323681379670446E-4</v>
       </c>
       <c r="M16" s="1">
-        <v>1.5214132735586053E-3</v>
+        <v>1.6198795199181746E-3</v>
       </c>
       <c r="N16" s="1">
-        <v>-2.8517345588757515E-3</v>
+        <v>-3.5837282167548502E-3</v>
       </c>
       <c r="O16" s="1">
-        <v>2.8507013697577528E-3</v>
+        <v>3.8787860703672246E-3</v>
       </c>
       <c r="P16" s="1">
-        <v>9.5873362745419622E-3</v>
+        <v>1.2201770726416802E-2</v>
       </c>
       <c r="Q16" s="1">
-        <v>0.11498449208889376</v>
+        <v>0.15124198306159731</v>
       </c>
       <c r="R16" s="1">
-        <v>0.85404709617325736</v>
+        <v>1.4066838369445118</v>
       </c>
       <c r="S16" s="1">
-        <v>1.0528903902766939E-3</v>
+        <v>1.0865329572318538E-3</v>
       </c>
       <c r="T16" s="1">
-        <v>2.3517058844245756E-3</v>
+        <v>2.0332635093037498E-3</v>
       </c>
       <c r="U16" s="1">
-        <v>14.894373487473009</v>
+        <v>18.298357988723396</v>
       </c>
       <c r="V16" s="1">
-        <v>1.3620663984584868E-3</v>
+        <v>2.7817256586549835E-3</v>
       </c>
       <c r="W16" s="1">
-        <v>-3.4691389208015656E-4</v>
+        <v>-4.7247340192309488E-3</v>
       </c>
       <c r="X16" s="1">
-        <v>4.4828932653077225E-4</v>
+        <v>3.701786603820369E-4</v>
       </c>
       <c r="Y16" s="1">
-        <v>6.8767064908112907E-2</v>
+        <v>0.13083350488817724</v>
       </c>
       <c r="Z16" s="1">
-        <v>0.18430166249340973</v>
+        <v>0.2993605849684482</v>
       </c>
       <c r="AA16" s="1">
-        <v>3.4691145174237725</v>
+        <v>3.1037118040608149</v>
       </c>
       <c r="AB16" s="1">
-        <v>3.0340490881591692E-3</v>
+        <v>3.0290022565030439E-3</v>
       </c>
       <c r="AC16" s="1">
-        <v>0.34453499239003743</v>
+        <v>0.35505870064081568</v>
       </c>
     </row>
     <row r="17" spans="1:29">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="3">
-        <v>7.97</v>
-      </c>
-      <c r="D17">
-        <v>136</v>
-      </c>
-      <c r="E17" s="2">
-        <v>4</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="E17" s="2"/>
       <c r="F17" s="3">
-        <v>51.43</v>
+        <v>51.3</v>
       </c>
       <c r="G17" s="1">
-        <v>0.13030325861004863</v>
+        <v>0.13062763769404137</v>
       </c>
       <c r="H17" s="1">
-        <v>-1.9243036335420927E-3</v>
+        <v>-7.954371749141915E-4</v>
       </c>
       <c r="I17" s="1">
-        <v>0.13984916284508361</v>
+        <v>0.13894282571997763</v>
       </c>
       <c r="J17" s="1">
-        <v>9.9867131154848687E-2</v>
+        <v>9.9859213313141251E-2</v>
       </c>
       <c r="K17" s="1">
-        <v>-1.6014814303847198E-4</v>
+        <v>-1.7529874516052143E-3</v>
       </c>
       <c r="L17" s="1">
-        <v>6.9323681379670446E-4</v>
+        <v>7.1448906604929961E-4</v>
       </c>
       <c r="M17" s="1">
-        <v>1.6198795199181746E-3</v>
+        <v>1.2016717393255416E-3</v>
       </c>
       <c r="N17" s="1">
-        <v>-3.5837282167548502E-3</v>
+        <v>-3.4952522864439214E-3</v>
       </c>
       <c r="O17" s="1">
-        <v>3.8787860703672246E-3</v>
+        <v>3.0063154100856064E-3</v>
       </c>
       <c r="P17" s="1">
-        <v>1.2201770726416802E-2</v>
+        <v>1.2045021820186602E-2</v>
       </c>
       <c r="Q17" s="1">
-        <v>0.15124198306159731</v>
+        <v>0.14987556900754481</v>
       </c>
       <c r="R17" s="1">
-        <v>1.4066838369445118</v>
+        <v>1.4024466305473151</v>
       </c>
       <c r="S17" s="1">
-        <v>1.0865329572318538E-3</v>
+        <v>1.2222298212975441E-3</v>
       </c>
       <c r="T17" s="1">
-        <v>2.0332635093037498E-3</v>
+        <v>3.5427828033019223E-3</v>
       </c>
       <c r="U17" s="1">
-        <v>18.298357988723396</v>
+        <v>18.204814415206183</v>
       </c>
       <c r="V17" s="1">
-        <v>2.7817256586549835E-3</v>
+        <v>2.8376670580997649E-3</v>
       </c>
       <c r="W17" s="1">
-        <v>-4.7247340192309488E-3</v>
+        <v>-1.607797092255661E-3</v>
       </c>
       <c r="X17" s="1">
-        <v>3.701786603820369E-4</v>
+        <v>3.2732441028460879E-4</v>
       </c>
       <c r="Y17" s="1">
-        <v>0.13083350488817724</v>
+        <v>0.12953043020212654</v>
       </c>
       <c r="Z17" s="1">
-        <v>0.2993605849684482</v>
+        <v>0.29701481349782982</v>
       </c>
       <c r="AA17" s="1">
-        <v>3.1037118040608149</v>
+        <v>3.089664370415607</v>
       </c>
       <c r="AB17" s="1">
-        <v>3.0290022565030439E-3</v>
+        <v>2.9648967566244743E-3</v>
       </c>
       <c r="AC17" s="1">
-        <v>0.35505870064081568</v>
+        <v>0.35047891965529399</v>
       </c>
     </row>
     <row r="18" spans="1:29">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="E18" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="C18" s="3">
+        <v>8.07</v>
+      </c>
+      <c r="D18">
+        <v>171</v>
+      </c>
+      <c r="E18" s="2">
+        <v>8</v>
+      </c>
       <c r="F18" s="3">
-        <v>51.3</v>
+        <v>56.82</v>
       </c>
       <c r="G18" s="1">
-        <v>0.13062763769404137</v>
+        <v>0.16229687596619821</v>
       </c>
       <c r="H18" s="1">
-        <v>-7.954371749141915E-4</v>
+        <v>1.9115141831134181E-5</v>
       </c>
       <c r="I18" s="1">
-        <v>0.13894282571997763</v>
+        <v>0.31575630391465076</v>
       </c>
       <c r="J18" s="1">
-        <v>9.9859213313141251E-2</v>
+        <v>0.13919187687884924</v>
       </c>
       <c r="K18" s="1">
-        <v>-1.7529874516052143E-3</v>
+        <v>-3.6984728419655727E-3</v>
       </c>
       <c r="L18" s="1">
-        <v>7.1448906604929961E-4</v>
+        <v>2.2918905285766239E-3</v>
       </c>
       <c r="M18" s="1">
-        <v>1.2016717393255416E-3</v>
+        <v>2.1642828991869853E-3</v>
       </c>
       <c r="N18" s="1">
-        <v>-3.4952522864439214E-3</v>
+        <v>-3.9453460016414177E-3</v>
       </c>
       <c r="O18" s="1">
-        <v>3.0063154100856064E-3</v>
+        <v>4.1318940346847461E-3</v>
       </c>
       <c r="P18" s="1">
-        <v>1.2045021820186602E-2</v>
+        <v>1.3451842959363816E-2</v>
       </c>
       <c r="Q18" s="1">
-        <v>0.14987556900754481</v>
+        <v>0.17252698533789146</v>
       </c>
       <c r="R18" s="1">
-        <v>1.4024466305473151</v>
+        <v>1.84958459276012</v>
       </c>
       <c r="S18" s="1">
-        <v>1.2222298212975441E-3</v>
+        <v>1.2198847646907689E-3</v>
       </c>
       <c r="T18" s="1">
-        <v>3.5427828033019223E-3</v>
+        <v>1.5038088531603045E-3</v>
       </c>
       <c r="U18" s="1">
-        <v>18.204814415206183</v>
+        <v>19.908487561729679</v>
       </c>
       <c r="V18" s="1">
-        <v>2.8376670580997649E-3</v>
+        <v>6.3561851187401647E-3</v>
       </c>
       <c r="W18" s="1">
-        <v>-1.607797092255661E-3</v>
+        <v>-2.2707756819993321E-3</v>
       </c>
       <c r="X18" s="1">
-        <v>3.2732441028460879E-4</v>
+        <v>4.0274183120742307E-4</v>
       </c>
       <c r="Y18" s="1">
-        <v>0.12953043020212654</v>
+        <v>0.28563598059414536</v>
       </c>
       <c r="Z18" s="1">
-        <v>0.29701481349782982</v>
+        <v>0.4251046207726808</v>
       </c>
       <c r="AA18" s="1">
-        <v>3.089664370415607</v>
+        <v>3.2083647153190795</v>
       </c>
       <c r="AB18" s="1">
-        <v>2.9648967566244743E-3</v>
+        <v>4.7952576439593058E-3</v>
       </c>
       <c r="AC18" s="1">
-        <v>0.35047891965529399</v>
+        <v>0.4223895789815198</v>
       </c>
     </row>
     <row r="19" spans="1:29">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" s="3">
-        <v>8.07</v>
-      </c>
-      <c r="D19">
-        <v>171</v>
-      </c>
-      <c r="E19" s="2">
-        <v>8</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="E19" s="2"/>
       <c r="F19" s="3">
-        <v>56.82</v>
+        <v>57.51</v>
       </c>
       <c r="G19" s="1">
-        <v>0.16229687596619821</v>
+        <v>0.16276112525958009</v>
       </c>
       <c r="H19" s="1">
-        <v>1.9115141831134181E-5</v>
+        <v>-2.3642185255545079E-3</v>
       </c>
       <c r="I19" s="1">
-        <v>0.31575630391465076</v>
+        <v>0.31629925717260404</v>
       </c>
       <c r="J19" s="1">
-        <v>0.13919187687884924</v>
+        <v>0.13885428787832774</v>
       </c>
       <c r="K19" s="1">
-        <v>-3.6984728419655727E-3</v>
+        <v>-1.3088898435803159E-4</v>
       </c>
       <c r="L19" s="1">
-        <v>2.2918905285766239E-3</v>
+        <v>2.2774642874974116E-3</v>
       </c>
       <c r="M19" s="1">
-        <v>2.1642828991869853E-3</v>
+        <v>2.2378015165663203E-3</v>
       </c>
       <c r="N19" s="1">
-        <v>-3.9453460016414177E-3</v>
+        <v>-4.3649376250088591E-3</v>
       </c>
       <c r="O19" s="1">
-        <v>4.1318940346847461E-3</v>
+        <v>5.3363541507416958E-3</v>
       </c>
       <c r="P19" s="1">
-        <v>1.3451842959363816E-2</v>
+        <v>1.3463550448208801E-2</v>
       </c>
       <c r="Q19" s="1">
-        <v>0.17252698533789146</v>
+        <v>0.17387370033453645</v>
       </c>
       <c r="R19" s="1">
-        <v>1.84958459276012</v>
+        <v>1.8424473262296843</v>
       </c>
       <c r="S19" s="1">
-        <v>1.2198847646907689E-3</v>
+        <v>1.2737731821089637E-3</v>
       </c>
       <c r="T19" s="1">
-        <v>1.5038088531603045E-3</v>
+        <v>1.8574041268252896E-3</v>
       </c>
       <c r="U19" s="1">
-        <v>19.908487561729679</v>
+        <v>19.955951952114525</v>
       </c>
       <c r="V19" s="1">
-        <v>6.3561851187401647E-3</v>
+        <v>6.3085414843518026E-3</v>
       </c>
       <c r="W19" s="1">
-        <v>-2.2707756819993321E-3</v>
+        <v>6.8369416929017974E-4</v>
       </c>
       <c r="X19" s="1">
-        <v>4.0274183120742307E-4</v>
+        <v>6.7456513130585954E-4</v>
       </c>
       <c r="Y19" s="1">
-        <v>0.28563598059414536</v>
+        <v>0.28636103882080349</v>
       </c>
       <c r="Z19" s="1">
-        <v>0.4251046207726808</v>
+        <v>0.42586508643421667</v>
       </c>
       <c r="AA19" s="1">
-        <v>3.2083647153190795</v>
+        <v>3.1909782362786756</v>
       </c>
       <c r="AB19" s="1">
-        <v>4.7952576439593058E-3</v>
+        <v>4.8761809359111905E-3</v>
       </c>
       <c r="AC19" s="1">
-        <v>0.4223895789815198</v>
+        <v>0.44461442386085198</v>
       </c>
     </row>
     <row r="20" spans="1:29">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="E20" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="C20" s="3">
+        <v>7.85</v>
+      </c>
+      <c r="D20">
+        <v>140</v>
+      </c>
+      <c r="E20" s="2">
+        <v>7</v>
+      </c>
       <c r="F20" s="3">
-        <v>57.51</v>
+        <v>54.43</v>
       </c>
       <c r="G20" s="1">
-        <v>0.16276112525958009</v>
+        <v>8.8876823378132699E-2</v>
       </c>
       <c r="H20" s="1">
-        <v>-2.3642185255545079E-3</v>
+        <v>-7.1172369548745771E-4</v>
       </c>
       <c r="I20" s="1">
-        <v>0.31629925717260404</v>
+        <v>6.0247339113981897E-2</v>
       </c>
       <c r="J20" s="1">
-        <v>0.13885428787832774</v>
+        <v>2.1414363725450049E-2</v>
       </c>
       <c r="K20" s="1">
-        <v>-1.3088898435803159E-4</v>
+        <v>-2.6636646087722995E-3</v>
       </c>
       <c r="L20" s="1">
-        <v>2.2774642874974116E-3</v>
+        <v>2.6032223189951574E-5</v>
       </c>
       <c r="M20" s="1">
-        <v>2.2378015165663203E-3</v>
+        <v>1.0772426705963768E-3</v>
       </c>
       <c r="N20" s="1">
-        <v>-4.3649376250088591E-3</v>
+        <v>-3.4158206929353553E-3</v>
       </c>
       <c r="O20" s="1">
-        <v>5.3363541507416958E-3</v>
+        <v>4.2929657580051172E-3</v>
       </c>
       <c r="P20" s="1">
-        <v>1.3463550448208801E-2</v>
+        <v>2.0591900275906318E-2</v>
       </c>
       <c r="Q20" s="1">
-        <v>0.17387370033453645</v>
+        <v>0.13355619070743602</v>
       </c>
       <c r="R20" s="1">
-        <v>1.8424473262296843</v>
+        <v>1.0140967823887388</v>
       </c>
       <c r="S20" s="1">
-        <v>1.2737731821089637E-3</v>
+        <v>1.1321672459904608E-3</v>
       </c>
       <c r="T20" s="1">
-        <v>1.8574041268252896E-3</v>
+        <v>1.5377347326597866E-3</v>
       </c>
       <c r="U20" s="1">
-        <v>19.955951952114525</v>
+        <v>20.095509055867556</v>
       </c>
       <c r="V20" s="1">
-        <v>6.3085414843518026E-3</v>
+        <v>3.4843634539847516E-3</v>
       </c>
       <c r="W20" s="1">
-        <v>6.8369416929017974E-4</v>
+        <v>-4.3576377054652132E-4</v>
       </c>
       <c r="X20" s="1">
-        <v>6.7456513130585954E-4</v>
+        <v>2.7042701492284823E-4</v>
       </c>
       <c r="Y20" s="1">
-        <v>0.28636103882080349</v>
+        <v>9.3719057901015493E-2</v>
       </c>
       <c r="Z20" s="1">
-        <v>0.42586508643421667</v>
+        <v>0.18287847470572827</v>
       </c>
       <c r="AA20" s="1">
-        <v>3.1909782362786756</v>
+        <v>3.5174405773499555</v>
       </c>
       <c r="AB20" s="1">
-        <v>4.8761809359111905E-3</v>
+        <v>1.6663379512812046E-3</v>
       </c>
       <c r="AC20" s="1">
-        <v>0.44461442386085198</v>
+        <v>0.33635515444184544</v>
       </c>
     </row>
     <row r="21" spans="1:29">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="3">
-        <v>7.85</v>
-      </c>
-      <c r="D21">
-        <v>140</v>
-      </c>
-      <c r="E21" s="2">
-        <v>7</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="E21" s="2"/>
       <c r="F21" s="3">
-        <v>54.43</v>
+        <v>53.95</v>
       </c>
       <c r="G21" s="1">
-        <v>8.8876823378132699E-2</v>
+        <v>9.1993178777393339E-2</v>
       </c>
       <c r="H21" s="1">
-        <v>-7.1172369548745771E-4</v>
+        <v>-2.1059659449073338E-3</v>
       </c>
       <c r="I21" s="1">
-        <v>6.0247339113981897E-2</v>
+        <v>6.0536859343560449E-2</v>
       </c>
       <c r="J21" s="1">
-        <v>2.1414363725450049E-2</v>
+        <v>2.1899474276615968E-2</v>
       </c>
       <c r="K21" s="1">
-        <v>-2.6636646087722995E-3</v>
+        <v>-2.0388339804600988E-3</v>
       </c>
       <c r="L21" s="1">
-        <v>2.6032223189951574E-5</v>
+        <v>2.1221772008163243E-4</v>
       </c>
       <c r="M21" s="1">
-        <v>1.0772426705963768E-3</v>
+        <v>7.9202093109092175E-4</v>
       </c>
       <c r="N21" s="1">
-        <v>-3.4158206929353553E-3</v>
+        <v>-2.9221350797282585E-3</v>
       </c>
       <c r="O21" s="1">
-        <v>4.2929657580051172E-3</v>
+        <v>2.5352821873035679E-3</v>
       </c>
       <c r="P21" s="1">
-        <v>2.0591900275906318E-2</v>
+        <v>2.0498961868141558E-2</v>
       </c>
       <c r="Q21" s="1">
-        <v>0.13355619070743602</v>
+        <v>0.13315977193040965</v>
       </c>
       <c r="R21" s="1">
-        <v>1.0140967823887388</v>
+        <v>1.0032416038429726</v>
       </c>
       <c r="S21" s="1">
-        <v>1.1321672459904608E-3</v>
+        <v>1.0779440892598241E-3</v>
       </c>
       <c r="T21" s="1">
-        <v>1.5377347326597866E-3</v>
+        <v>3.5711404795540844E-3</v>
       </c>
       <c r="U21" s="1">
-        <v>20.095509055867556</v>
+        <v>19.911125816018814</v>
       </c>
       <c r="V21" s="1">
-        <v>3.4843634539847516E-3</v>
+        <v>3.5866939423928441E-3</v>
       </c>
       <c r="W21" s="1">
-        <v>-4.3576377054652132E-4</v>
+        <v>-3.9951924010942575E-3</v>
       </c>
       <c r="X21" s="1">
-        <v>2.7042701492284823E-4</v>
+        <v>3.7865535915829353E-4</v>
       </c>
       <c r="Y21" s="1">
-        <v>9.3719057901015493E-2</v>
+        <v>9.3127444523800618E-2</v>
       </c>
       <c r="Z21" s="1">
-        <v>0.18287847470572827</v>
+        <v>0.18184897711720291</v>
       </c>
       <c r="AA21" s="1">
-        <v>3.5174405773499555</v>
+        <v>3.4881296219482452</v>
       </c>
       <c r="AB21" s="1">
-        <v>1.6663379512812046E-3</v>
+        <v>1.6036239684993209E-3</v>
       </c>
       <c r="AC21" s="1">
-        <v>0.33635515444184544</v>
+        <v>0.32131930470725206</v>
       </c>
     </row>
     <row r="22" spans="1:29">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="E22" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="C22" s="3">
+        <v>7.67</v>
+      </c>
+      <c r="D22">
+        <v>146</v>
+      </c>
+      <c r="E22" s="2">
+        <v>7</v>
+      </c>
       <c r="F22" s="3">
-        <v>53.95</v>
+        <v>56.82</v>
       </c>
       <c r="G22" s="1">
-        <v>9.1993178777393339E-2</v>
+        <v>0.16419897475704848</v>
       </c>
       <c r="H22" s="1">
-        <v>-2.1059659449073338E-3</v>
+        <v>-2.0622664690787738E-3</v>
       </c>
       <c r="I22" s="1">
-        <v>6.0536859343560449E-2</v>
+        <v>0.29339716368060448</v>
       </c>
       <c r="J22" s="1">
-        <v>2.1899474276615968E-2</v>
+        <v>0.12466067593503775</v>
       </c>
       <c r="K22" s="1">
-        <v>-2.0388339804600988E-3</v>
+        <v>-2.1773273427328093E-3</v>
       </c>
       <c r="L22" s="1">
-        <v>2.1221772008163243E-4</v>
+        <v>1.8395184588450714E-3</v>
       </c>
       <c r="M22" s="1">
-        <v>7.9202093109092175E-4</v>
+        <v>1.7852934379962507E-3</v>
       </c>
       <c r="N22" s="1">
-        <v>-2.9221350797282585E-3</v>
+        <v>-5.5203749869770389E-3</v>
       </c>
       <c r="O22" s="1">
-        <v>2.5352821873035679E-3</v>
+        <v>5.4327713410446269E-3</v>
       </c>
       <c r="P22" s="1">
-        <v>2.0498961868141558E-2</v>
+        <v>1.2985601954989275E-2</v>
       </c>
       <c r="Q22" s="1">
-        <v>0.13315977193040965</v>
+        <v>0.21875132172729495</v>
       </c>
       <c r="R22" s="1">
-        <v>1.0032416038429726</v>
+        <v>1.7557059405019952</v>
       </c>
       <c r="S22" s="1">
-        <v>1.0779440892598241E-3</v>
+        <v>1.2971847138095107E-3</v>
       </c>
       <c r="T22" s="1">
-        <v>3.5711404795540844E-3</v>
+        <v>3.5386087507122328E-3</v>
       </c>
       <c r="U22" s="1">
-        <v>19.911125816018814</v>
+        <v>19.85910924770285</v>
       </c>
       <c r="V22" s="1">
-        <v>3.5866939423928441E-3</v>
+        <v>6.5853163826087649E-3</v>
       </c>
       <c r="W22" s="1">
-        <v>-3.9951924010942575E-3</v>
+        <v>-3.9968712424991761E-3</v>
       </c>
       <c r="X22" s="1">
-        <v>3.7865535915829353E-4</v>
+        <v>4.769699374258391E-4</v>
       </c>
       <c r="Y22" s="1">
-        <v>9.3127444523800618E-2</v>
+        <v>0.26460742536893228</v>
       </c>
       <c r="Z22" s="1">
-        <v>0.18184897711720291</v>
+        <v>0.40380307888543204</v>
       </c>
       <c r="AA22" s="1">
-        <v>3.4881296219482452</v>
+        <v>3.1853335795446989</v>
       </c>
       <c r="AB22" s="1">
-        <v>1.6036239684993209E-3</v>
+        <v>4.4960262226299034E-3</v>
       </c>
       <c r="AC22" s="1">
-        <v>0.32131930470725206</v>
+        <v>0.41864740215552976</v>
       </c>
     </row>
     <row r="23" spans="1:29">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="3">
-        <v>7.67</v>
-      </c>
-      <c r="D23">
-        <v>146</v>
-      </c>
-      <c r="E23" s="2">
-        <v>7</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="E23" s="2"/>
       <c r="F23" s="3">
-        <v>56.82</v>
+        <v>56.54</v>
       </c>
       <c r="G23" s="1">
-        <v>0.16419897475704848</v>
+        <v>0.16861069528613462</v>
       </c>
       <c r="H23" s="1">
-        <v>-2.0622664690787738E-3</v>
+        <v>-1.6491017783946571E-3</v>
       </c>
       <c r="I23" s="1">
-        <v>0.29339716368060448</v>
+        <v>0.29334631554875484</v>
       </c>
       <c r="J23" s="1">
-        <v>0.12466067593503775</v>
+        <v>0.12617204849718733</v>
       </c>
       <c r="K23" s="1">
-        <v>-2.1773273427328093E-3</v>
+        <v>1.0359138503749333E-3</v>
       </c>
       <c r="L23" s="1">
-        <v>1.8395184588450714E-3</v>
+        <v>2.118828596064284E-3</v>
       </c>
       <c r="M23" s="1">
-        <v>1.7852934379962507E-3</v>
+        <v>2.3062991885753645E-3</v>
       </c>
       <c r="N23" s="1">
-        <v>-5.5203749869770389E-3</v>
+        <v>-5.2046213872677374E-3</v>
       </c>
       <c r="O23" s="1">
-        <v>5.4327713410446269E-3</v>
+        <v>4.0942864881524871E-3</v>
       </c>
       <c r="P23" s="1">
-        <v>1.2985601954989275E-2</v>
+        <v>1.2963500182338128E-2</v>
       </c>
       <c r="Q23" s="1">
-        <v>0.21875132172729495</v>
+        <v>0.2176974709749423</v>
       </c>
       <c r="R23" s="1">
-        <v>1.7557059405019952</v>
+        <v>1.7496947005912704</v>
       </c>
       <c r="S23" s="1">
-        <v>1.2971847138095107E-3</v>
+        <v>1.1074709611047044E-3</v>
       </c>
       <c r="T23" s="1">
-        <v>3.5386087507122328E-3</v>
+        <v>2.3513945945962318E-3</v>
       </c>
       <c r="U23" s="1">
-        <v>19.85910924770285</v>
+        <v>19.789518550831787</v>
       </c>
       <c r="V23" s="1">
-        <v>6.5853163826087649E-3</v>
+        <v>6.5176337457548235E-3</v>
       </c>
       <c r="W23" s="1">
-        <v>-3.9968712424991761E-3</v>
+        <v>-9.3618914711087093E-4</v>
       </c>
       <c r="X23" s="1">
-        <v>4.769699374258391E-4</v>
+        <v>5.0665259445923814E-4</v>
       </c>
       <c r="Y23" s="1">
-        <v>0.26460742536893228</v>
+        <v>0.26351462624782124</v>
       </c>
       <c r="Z23" s="1">
-        <v>0.40380307888543204</v>
+        <v>0.40398971926415578</v>
       </c>
       <c r="AA23" s="1">
-        <v>3.1853335795446989</v>
+        <v>3.1982044305753186</v>
       </c>
       <c r="AB23" s="1">
-        <v>4.4960262226299034E-3</v>
+        <v>4.424552648681598E-3</v>
       </c>
       <c r="AC23" s="1">
-        <v>0.41864740215552976</v>
+        <v>0.40535142151142756</v>
       </c>
     </row>
     <row r="24" spans="1:29">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="E24" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="C24" s="3">
+        <v>8.07</v>
+      </c>
+      <c r="D24">
+        <v>154</v>
+      </c>
+      <c r="E24" s="2">
+        <v>4</v>
+      </c>
       <c r="F24" s="3">
-        <v>56.54</v>
+        <v>61.61</v>
       </c>
       <c r="G24" s="1">
-        <v>0.16861069528613462</v>
+        <v>0.12006571345440652</v>
       </c>
       <c r="H24" s="1">
-        <v>-1.6491017783946571E-3</v>
+        <v>-1.8821228414374379E-3</v>
       </c>
       <c r="I24" s="1">
-        <v>0.29334631554875484</v>
+        <v>0.19621418724300477</v>
       </c>
       <c r="J24" s="1">
-        <v>0.12617204849718733</v>
+        <v>9.5548582117970571E-2</v>
       </c>
       <c r="K24" s="1">
-        <v>1.0359138503749333E-3</v>
+        <v>1.4206408831280598E-4</v>
       </c>
       <c r="L24" s="1">
-        <v>2.118828596064284E-3</v>
+        <v>1.3359157289718809E-3</v>
       </c>
       <c r="M24" s="1">
-        <v>2.3062991885753645E-3</v>
+        <v>1.5202861648972658E-3</v>
       </c>
       <c r="N24" s="1">
-        <v>-5.2046213872677374E-3</v>
+        <v>-5.3675430791699412E-3</v>
       </c>
       <c r="O24" s="1">
-        <v>4.0942864881524871E-3</v>
+        <v>3.698038116124213E-3</v>
       </c>
       <c r="P24" s="1">
-        <v>1.2963500182338128E-2</v>
+        <v>9.63040512489397E-3</v>
       </c>
       <c r="Q24" s="1">
-        <v>0.2176974709749423</v>
+        <v>0.21732525823808968</v>
       </c>
       <c r="R24" s="1">
-        <v>1.7496947005912704</v>
+        <v>1.731684103696381</v>
       </c>
       <c r="S24" s="1">
-        <v>1.1074709611047044E-3</v>
+        <v>1.120907600409777E-3</v>
       </c>
       <c r="T24" s="1">
-        <v>2.3513945945962318E-3</v>
+        <v>5.0537213306137479E-3</v>
       </c>
       <c r="U24" s="1">
-        <v>19.789518550831787</v>
+        <v>21.829152567404154</v>
       </c>
       <c r="V24" s="1">
-        <v>6.5176337457548235E-3</v>
+        <v>6.7750792366029697E-3</v>
       </c>
       <c r="W24" s="1">
-        <v>-9.3618914711087093E-4</v>
+        <v>-3.0035728013051138E-3</v>
       </c>
       <c r="X24" s="1">
-        <v>5.0665259445923814E-4</v>
+        <v>-1.4318874057570407E-4</v>
       </c>
       <c r="Y24" s="1">
-        <v>0.26351462624782124</v>
+        <v>0.24781906700244441</v>
       </c>
       <c r="Z24" s="1">
-        <v>0.40398971926415578</v>
+        <v>0.66499285036841538</v>
       </c>
       <c r="AA24" s="1">
-        <v>3.1982044305753186</v>
+        <v>3.2856354145796147</v>
       </c>
       <c r="AB24" s="1">
-        <v>4.424552648681598E-3</v>
+        <v>3.6682241532817622E-3</v>
       </c>
       <c r="AC24" s="1">
-        <v>0.40535142151142756</v>
+        <v>0.41035289220967092</v>
       </c>
     </row>
     <row r="25" spans="1:29">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="3">
-        <v>8.07</v>
-      </c>
-      <c r="D25">
-        <v>154</v>
-      </c>
-      <c r="E25" s="2">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="F25" s="3">
-        <v>61.61</v>
+        <v>61.37</v>
       </c>
       <c r="G25" s="1">
-        <v>0.12006571345440652</v>
+        <v>0.11772719391791397</v>
       </c>
       <c r="H25" s="1">
-        <v>-1.8821228414374379E-3</v>
+        <v>-4.7072504837874975E-4</v>
       </c>
       <c r="I25" s="1">
-        <v>0.19621418724300477</v>
+        <v>0.19607437365637867</v>
       </c>
       <c r="J25" s="1">
-        <v>9.5548582117970571E-2</v>
+        <v>9.5121810635762416E-2</v>
       </c>
       <c r="K25" s="1">
-        <v>1.4206408831280598E-4</v>
+        <v>1.0439775964830491E-3</v>
       </c>
       <c r="L25" s="1">
-        <v>1.3359157289718809E-3</v>
+        <v>1.3141110042351088E-3</v>
       </c>
       <c r="M25" s="1">
-        <v>1.5202861648972658E-3</v>
+        <v>1.5171910958758483E-3</v>
       </c>
       <c r="N25" s="1">
-        <v>-5.3675430791699412E-3</v>
+        <v>-5.3809379091899019E-3</v>
       </c>
       <c r="O25" s="1">
-        <v>3.698038116124213E-3</v>
+        <v>4.8493408795176633E-3</v>
       </c>
       <c r="P25" s="1">
-        <v>9.63040512489397E-3</v>
+        <v>9.6740670584205251E-3</v>
       </c>
       <c r="Q25" s="1">
-        <v>0.21732525823808968</v>
+        <v>0.21713560345693747</v>
       </c>
       <c r="R25" s="1">
-        <v>1.731684103696381</v>
+        <v>1.7245071924235253</v>
       </c>
       <c r="S25" s="1">
-        <v>1.120907600409777E-3</v>
+        <v>1.1852133972158202E-3</v>
       </c>
       <c r="T25" s="1">
-        <v>5.0537213306137479E-3</v>
+        <v>2.3903794438475691E-3</v>
       </c>
       <c r="U25" s="1">
-        <v>21.829152567404154</v>
+        <v>21.758275840977465</v>
       </c>
       <c r="V25" s="1">
-        <v>6.7750792366029697E-3</v>
+        <v>6.8790844083242699E-3</v>
       </c>
       <c r="W25" s="1">
-        <v>-3.0035728013051138E-3</v>
+        <v>-2.2447956833275989E-3</v>
       </c>
       <c r="X25" s="1">
-        <v>-1.4318874057570407E-4</v>
+        <v>5.5146402230830179E-4</v>
       </c>
       <c r="Y25" s="1">
-        <v>0.24781906700244441</v>
+        <v>0.24821935104014506</v>
       </c>
       <c r="Z25" s="1">
-        <v>0.66499285036841538</v>
+        <v>0.66263941347266286</v>
       </c>
       <c r="AA25" s="1">
-        <v>3.2856354145796147</v>
+        <v>3.2793299498634085</v>
       </c>
       <c r="AB25" s="1">
-        <v>3.6682241532817622E-3</v>
+        <v>3.7128506346610743E-3</v>
       </c>
       <c r="AC25" s="1">
-        <v>0.41035289220967092</v>
+        <v>0.42378536123488825</v>
       </c>
     </row>
     <row r="26" spans="1:29">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="F26" s="3">
-        <v>61.37</v>
-      </c>
-      <c r="G26" s="1">
-        <v>0.11772719391791397</v>
-      </c>
-      <c r="H26" s="1">
-        <v>-4.7072504837874975E-4</v>
-      </c>
-      <c r="I26" s="1">
-        <v>0.19607437365637867</v>
-      </c>
-      <c r="J26" s="1">
-        <v>9.5121810635762416E-2</v>
-      </c>
-      <c r="K26" s="1">
-        <v>1.0439775964830491E-3</v>
-      </c>
-      <c r="L26" s="1">
-        <v>1.3141110042351088E-3</v>
-      </c>
-      <c r="M26" s="1">
-        <v>1.5171910958758483E-3</v>
-      </c>
-      <c r="N26" s="1">
-        <v>-5.3809379091899019E-3</v>
-      </c>
-      <c r="O26" s="1">
-        <v>4.8493408795176633E-3</v>
-      </c>
-      <c r="P26" s="1">
-        <v>9.6740670584205251E-3</v>
-      </c>
-      <c r="Q26" s="1">
-        <v>0.21713560345693747</v>
-      </c>
-      <c r="R26" s="1">
-        <v>1.7245071924235253</v>
-      </c>
-      <c r="S26" s="1">
-        <v>1.1852133972158202E-3</v>
-      </c>
-      <c r="T26" s="1">
-        <v>2.3903794438475691E-3</v>
-      </c>
-      <c r="U26" s="1">
-        <v>21.758275840977465</v>
-      </c>
-      <c r="V26" s="1">
-        <v>6.8790844083242699E-3</v>
-      </c>
-      <c r="W26" s="1">
-        <v>-2.2447956833275989E-3</v>
-      </c>
-      <c r="X26" s="1">
-        <v>5.5146402230830179E-4</v>
-      </c>
-      <c r="Y26" s="1">
-        <v>0.24821935104014506</v>
-      </c>
-      <c r="Z26" s="1">
-        <v>0.66263941347266286</v>
-      </c>
-      <c r="AA26" s="1">
-        <v>3.2793299498634085</v>
-      </c>
-      <c r="AB26" s="1">
-        <v>3.7128506346610743E-3</v>
-      </c>
-      <c r="AC26" s="1">
-        <v>0.42378536123488825</v>
+        <v>62</v>
+      </c>
+      <c r="C26">
+        <v>8.44</v>
+      </c>
+      <c r="D26">
+        <v>275</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>107.2</v>
+      </c>
+      <c r="G26">
+        <v>1.4519834722366516E-2</v>
+      </c>
+      <c r="H26" t="s">
+        <v>60</v>
+      </c>
+      <c r="I26">
+        <v>3.141288075912007E-2</v>
+      </c>
+      <c r="J26">
+        <v>-2.7784294155941663E-4</v>
+      </c>
+      <c r="K26">
+        <v>3.818578405303761E-3</v>
+      </c>
+      <c r="L26">
+        <v>2.5776106933446196E-4</v>
+      </c>
+      <c r="M26">
+        <v>9.5509343718654354E-4</v>
+      </c>
+      <c r="N26">
+        <v>-1.1361860069156284E-3</v>
+      </c>
+      <c r="O26">
+        <v>1.2696203595613907E-2</v>
+      </c>
+      <c r="P26">
+        <v>1.2590162084309272E-2</v>
+      </c>
+      <c r="Q26">
+        <v>4.9798999253114255E-2</v>
+      </c>
+      <c r="R26">
+        <v>3.8851999984140435</v>
+      </c>
+      <c r="S26">
+        <v>2.6714075411480171E-4</v>
+      </c>
+      <c r="T26">
+        <v>9.4615441134544701E-4</v>
+      </c>
+      <c r="U26">
+        <v>37.705876849295322</v>
+      </c>
+      <c r="V26">
+        <v>7.1302443525957354E-4</v>
+      </c>
+      <c r="W26">
+        <v>-6.595992772925636E-3</v>
+      </c>
+      <c r="X26">
+        <v>5.7730300257611705E-6</v>
+      </c>
+      <c r="Y26">
+        <v>0.24389979886607335</v>
+      </c>
+      <c r="Z26">
+        <v>0.19652057807062792</v>
+      </c>
+      <c r="AA26">
+        <v>6.3742068091220423</v>
+      </c>
+      <c r="AB26">
+        <v>5.0107550195484926E-3</v>
+      </c>
+      <c r="AC26">
+        <v>1.038546674777483</v>
       </c>
     </row>
     <row r="27" spans="1:29">
@@ -3449,88 +3406,82 @@
         <v>52</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27">
-        <v>8.44</v>
-      </c>
-      <c r="D27">
-        <v>275</v>
-      </c>
-      <c r="E27">
-        <v>2</v>
-      </c>
-      <c r="F27">
-        <v>107.2</v>
+        <v>62</v>
+      </c>
+      <c r="E27" s="2">
+        <v>5</v>
+      </c>
+      <c r="F27" s="4">
+        <v>106.4</v>
       </c>
       <c r="G27">
-        <v>1.4519834722366516E-2</v>
-      </c>
-      <c r="H27" t="s">
-        <v>61</v>
+        <v>1.4796683157488675E-2</v>
+      </c>
+      <c r="H27">
+        <v>5.5523308668632601E-4</v>
       </c>
       <c r="I27">
-        <v>3.141288075912007E-2</v>
+        <v>3.1535217868645708E-2</v>
       </c>
       <c r="J27">
-        <v>-2.7784294155941663E-4</v>
+        <v>1.8792589038318748E-4</v>
       </c>
       <c r="K27">
-        <v>3.818578405303761E-3</v>
+        <v>6.6061069624917153E-3</v>
       </c>
       <c r="L27">
-        <v>2.5776106933446196E-4</v>
+        <v>2.3933831217064485E-4</v>
       </c>
       <c r="M27">
-        <v>9.5509343718654354E-4</v>
+        <v>1.0632643703235827E-3</v>
       </c>
       <c r="N27">
-        <v>-1.1361860069156284E-3</v>
+        <v>-1.3695121137386964E-3</v>
       </c>
       <c r="O27">
-        <v>1.2696203595613907E-2</v>
+        <v>1.1471792819167959E-2</v>
       </c>
       <c r="P27">
-        <v>1.2590162084309272E-2</v>
+        <v>1.2420238237200875E-2</v>
       </c>
       <c r="Q27">
-        <v>4.9798999253114255E-2</v>
+        <v>4.8194567727197789E-2</v>
       </c>
       <c r="R27">
-        <v>3.8851999984140435</v>
+        <v>3.8788538200439451</v>
       </c>
       <c r="S27">
-        <v>2.6714075411480171E-4</v>
+        <v>-3.00773481021856E-5</v>
       </c>
       <c r="T27">
-        <v>9.4615441134544701E-4</v>
+        <v>1.1196917181786391E-3</v>
       </c>
       <c r="U27">
-        <v>37.705876849295322</v>
+        <v>37.33436669808232</v>
       </c>
       <c r="V27">
-        <v>7.1302443525957354E-4</v>
+        <v>3.7731817945190724E-4</v>
       </c>
       <c r="W27">
-        <v>-6.595992772925636E-3</v>
+        <v>-8.9940471434331194E-3</v>
       </c>
       <c r="X27">
-        <v>5.7730300257611705E-6</v>
+        <v>2.1290656940126381E-4</v>
       </c>
       <c r="Y27">
-        <v>0.24389979886607335</v>
+        <v>0.24130116096795587</v>
       </c>
       <c r="Z27">
-        <v>0.19652057807062792</v>
+        <v>0.19598388642231393</v>
       </c>
       <c r="AA27">
-        <v>6.3742068091220423</v>
+        <v>6.2901958197564865</v>
       </c>
       <c r="AB27">
-        <v>5.0107550195484926E-3</v>
+        <v>4.96875971480482E-3</v>
       </c>
       <c r="AC27">
-        <v>1.038546674777483</v>
+        <v>1.0237230715347829</v>
       </c>
     </row>
     <row r="28" spans="1:29">
@@ -3538,82 +3489,88 @@
         <v>53</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" s="2">
-        <v>5</v>
+        <v>63</v>
+      </c>
+      <c r="C28">
+        <v>8.32</v>
+      </c>
+      <c r="D28">
+        <v>238</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
       </c>
       <c r="F28" s="4">
-        <v>106.4</v>
+        <v>84.27</v>
       </c>
       <c r="G28">
-        <v>1.4796683157488675E-2</v>
+        <v>2.2010406368870122E-2</v>
       </c>
       <c r="H28">
-        <v>5.5523308668632601E-4</v>
+        <v>1.0063906037402536E-3</v>
       </c>
       <c r="I28">
-        <v>3.1535217868645708E-2</v>
+        <v>8.6969683060961075E-2</v>
       </c>
       <c r="J28">
-        <v>1.8792589038318748E-4</v>
+        <v>9.1198843605166686E-3</v>
       </c>
       <c r="K28">
-        <v>6.6061069624917153E-3</v>
+        <v>5.606524984502992E-3</v>
       </c>
       <c r="L28">
-        <v>2.3933831217064485E-4</v>
+        <v>8.3618155061216564E-4</v>
       </c>
       <c r="M28">
-        <v>1.0632643703235827E-3</v>
+        <v>4.2230404871618931E-4</v>
       </c>
       <c r="N28">
-        <v>-1.3695121137386964E-3</v>
+        <v>-7.8784064790883882E-4</v>
       </c>
       <c r="O28">
-        <v>1.1471792819167959E-2</v>
+        <v>7.7998344298882104E-3</v>
       </c>
       <c r="P28">
-        <v>1.2420238237200875E-2</v>
+        <v>6.3978550015900268E-4</v>
       </c>
       <c r="Q28">
-        <v>4.8194567727197789E-2</v>
+        <v>1.4463865415730822E-2</v>
       </c>
       <c r="R28">
-        <v>3.8788538200439451</v>
+        <v>3.2214998570845292</v>
       </c>
       <c r="S28">
-        <v>-3.00773481021856E-5</v>
+        <v>1.3554222995602294E-5</v>
       </c>
       <c r="T28">
-        <v>1.1196917181786391E-3</v>
+        <v>-2.125681265627359E-3</v>
       </c>
       <c r="U28">
-        <v>37.33436669808232</v>
+        <v>33.972692803004065</v>
       </c>
       <c r="V28">
-        <v>3.7731817945190724E-4</v>
+        <v>5.6409468301960735E-4</v>
       </c>
       <c r="W28">
-        <v>-8.9940471434331194E-3</v>
+        <v>-7.7569877184853198E-3</v>
       </c>
       <c r="X28">
-        <v>2.1290656940126381E-4</v>
+        <v>2.9892598532616421E-4</v>
       </c>
       <c r="Y28">
-        <v>0.24130116096795587</v>
+        <v>0.30040720542729565</v>
       </c>
       <c r="Z28">
-        <v>0.19598388642231393</v>
+        <v>1.0552150044979465</v>
       </c>
       <c r="AA28">
-        <v>6.2901958197564865</v>
+        <v>4.2612965716387743</v>
       </c>
       <c r="AB28">
-        <v>4.96875971480482E-3</v>
+        <v>3.5930461625108523E-3</v>
       </c>
       <c r="AC28">
-        <v>1.0237230715347829</v>
+        <v>0.56334451769216765</v>
       </c>
     </row>
     <row r="29" spans="1:29">
@@ -3621,88 +3578,82 @@
         <v>54</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29">
-        <v>8.32</v>
-      </c>
-      <c r="D29">
-        <v>238</v>
+        <v>63</v>
       </c>
       <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29" s="4">
-        <v>84.27</v>
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>89.6</v>
       </c>
       <c r="G29">
-        <v>2.2010406368870122E-2</v>
+        <v>2.1890189737381466E-2</v>
       </c>
       <c r="H29">
-        <v>1.0063906037402536E-3</v>
+        <v>-1.8024570000536156E-5</v>
       </c>
       <c r="I29">
-        <v>8.6969683060961075E-2</v>
+        <v>8.7095037253088592E-2</v>
       </c>
       <c r="J29">
-        <v>9.1198843605166686E-3</v>
+        <v>1.0039028870199826E-2</v>
       </c>
       <c r="K29">
-        <v>5.606524984502992E-3</v>
+        <v>8.346472781099061E-3</v>
       </c>
       <c r="L29">
-        <v>8.3618155061216564E-4</v>
+        <v>8.0072662772874082E-4</v>
       </c>
       <c r="M29">
-        <v>4.2230404871618931E-4</v>
+        <v>5.885560022285052E-4</v>
       </c>
       <c r="N29">
-        <v>-7.8784064790883882E-4</v>
+        <v>-4.9450083787593924E-4</v>
       </c>
       <c r="O29">
-        <v>7.7998344298882104E-3</v>
+        <v>6.9792921654462346E-3</v>
       </c>
       <c r="P29">
-        <v>6.3978550015900268E-4</v>
+        <v>7.0079371651606177E-4</v>
       </c>
       <c r="Q29">
-        <v>1.4463865415730822E-2</v>
+        <v>1.4148201199317685E-2</v>
       </c>
       <c r="R29">
-        <v>3.2214998570845292</v>
+        <v>3.1991176061948998</v>
       </c>
       <c r="S29">
-        <v>1.3554222995602294E-5</v>
+        <v>1.3839091410209454E-4</v>
       </c>
       <c r="T29">
-        <v>-2.125681265627359E-3</v>
+        <v>-1.3577282266223083E-3</v>
       </c>
       <c r="U29">
-        <v>33.972692803004065</v>
+        <v>33.613125988577004</v>
       </c>
       <c r="V29">
-        <v>5.6409468301960735E-4</v>
+        <v>5.7566250316694702E-4</v>
       </c>
       <c r="W29">
-        <v>-7.7569877184853198E-3</v>
+        <v>-6.5192604435029347E-3</v>
       </c>
       <c r="X29">
-        <v>2.9892598532616421E-4</v>
+        <v>-4.1781288211662263E-4</v>
       </c>
       <c r="Y29">
-        <v>0.30040720542729565</v>
+        <v>0.29777857028492005</v>
       </c>
       <c r="Z29">
-        <v>1.0552150044979465</v>
+        <v>1.0538470290011033</v>
       </c>
       <c r="AA29">
-        <v>4.2612965716387743</v>
+        <v>4.1896611731976376</v>
       </c>
       <c r="AB29">
-        <v>3.5930461625108523E-3</v>
+        <v>3.6021383198760778E-3</v>
       </c>
       <c r="AC29">
-        <v>0.56334451769216765</v>
+        <v>0.55920390395908881</v>
       </c>
     </row>
     <row r="30" spans="1:29">
@@ -3710,82 +3661,88 @@
         <v>55</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
+      </c>
+      <c r="C30">
+        <v>8.56</v>
+      </c>
+      <c r="D30">
+        <v>270</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30">
-        <v>89.6</v>
+        <v>98.4</v>
       </c>
       <c r="G30">
-        <v>2.1890189737381466E-2</v>
+        <v>1.3413367202334185E-2</v>
       </c>
       <c r="H30">
-        <v>-1.8024570000536156E-5</v>
+        <v>9.8234027136905413E-4</v>
       </c>
       <c r="I30">
-        <v>8.7095037253088592E-2</v>
+        <v>3.4044375388665678E-2</v>
       </c>
       <c r="J30">
-        <v>1.0039028870199826E-2</v>
+        <v>1.337425067990651E-3</v>
       </c>
       <c r="K30">
-        <v>8.346472781099061E-3</v>
+        <v>5.0279923127811354E-3</v>
       </c>
       <c r="L30">
-        <v>8.0072662772874082E-4</v>
+        <v>3.4661237412569515E-4</v>
       </c>
       <c r="M30">
-        <v>5.885560022285052E-4</v>
+        <v>9.6948280395473473E-4</v>
       </c>
       <c r="N30">
-        <v>-4.9450083787593924E-4</v>
+        <v>-1.1244445662360505E-3</v>
       </c>
       <c r="O30">
-        <v>6.9792921654462346E-3</v>
+        <v>1.2089837864646001E-2</v>
       </c>
       <c r="P30">
-        <v>7.0079371651606177E-4</v>
+        <v>1.2296251280184328E-2</v>
       </c>
       <c r="Q30">
-        <v>1.4148201199317685E-2</v>
+        <v>3.8800983735783369E-2</v>
       </c>
       <c r="R30">
-        <v>3.1991176061948998</v>
+        <v>3.7521650704764311</v>
       </c>
       <c r="S30">
-        <v>1.3839091410209454E-4</v>
+        <v>1.6837636985925209E-4</v>
       </c>
       <c r="T30">
-        <v>-1.3577282266223083E-3</v>
+        <v>6.9837372756850584E-4</v>
       </c>
       <c r="U30">
-        <v>33.613125988577004</v>
+        <v>36.892689311420504</v>
       </c>
       <c r="V30">
-        <v>5.7566250316694702E-4</v>
+        <v>1.883972924968021E-3</v>
       </c>
       <c r="W30">
-        <v>-6.5192604435029347E-3</v>
+        <v>-3.5781963579337803E-3</v>
       </c>
       <c r="X30">
-        <v>-4.1781288211662263E-4</v>
+        <v>-5.0136768909181411E-5</v>
       </c>
       <c r="Y30">
-        <v>0.29777857028492005</v>
+        <v>0.25351074069423513</v>
       </c>
       <c r="Z30">
-        <v>1.0538470290011033</v>
+        <v>0.31438042906088132</v>
       </c>
       <c r="AA30">
-        <v>4.1896611731976376</v>
+        <v>5.9667827874250108</v>
       </c>
       <c r="AB30">
-        <v>3.6021383198760778E-3</v>
+        <v>4.9102283394016162E-3</v>
       </c>
       <c r="AC30">
-        <v>0.55920390395908881</v>
+        <v>0.86351572831676959</v>
       </c>
     </row>
     <row r="31" spans="1:29">
@@ -3793,88 +3750,82 @@
         <v>56</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31">
-        <v>8.56</v>
-      </c>
-      <c r="D31">
-        <v>270</v>
+        <v>61</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F31">
-        <v>98.4</v>
+        <v>98.2</v>
       </c>
       <c r="G31">
-        <v>1.3413367202334185E-2</v>
+        <v>1.309214800959835E-2</v>
       </c>
       <c r="H31">
-        <v>9.8234027136905413E-4</v>
+        <v>-3.3001582913460881E-4</v>
       </c>
       <c r="I31">
-        <v>3.4044375388665678E-2</v>
+        <v>3.446120782596767E-2</v>
       </c>
       <c r="J31">
-        <v>1.337425067990651E-3</v>
+        <v>9.3543411070398132E-4</v>
       </c>
       <c r="K31">
-        <v>5.0279923127811354E-3</v>
+        <v>8.7347545773524722E-3</v>
       </c>
       <c r="L31">
-        <v>3.4661237412569515E-4</v>
+        <v>2.1363142359214884E-4</v>
       </c>
       <c r="M31">
-        <v>9.6948280395473473E-4</v>
+        <v>9.837417580758174E-4</v>
       </c>
       <c r="N31">
-        <v>-1.1244445662360505E-3</v>
+        <v>-1.218196762588215E-3</v>
       </c>
       <c r="O31">
-        <v>1.2089837864646001E-2</v>
+        <v>1.1301597764670435E-2</v>
       </c>
       <c r="P31">
-        <v>1.2296251280184328E-2</v>
+        <v>1.2325395052518692E-2</v>
       </c>
       <c r="Q31">
-        <v>3.8800983735783369E-2</v>
+        <v>3.8276226482278318E-2</v>
       </c>
       <c r="R31">
-        <v>3.7521650704764311</v>
+        <v>3.7260431956336935</v>
       </c>
       <c r="S31">
-        <v>1.6837636985925209E-4</v>
+        <v>2.0153723381740587E-4</v>
       </c>
       <c r="T31">
-        <v>6.9837372756850584E-4</v>
+        <v>-6.6150579052835605E-4</v>
       </c>
       <c r="U31">
-        <v>36.892689311420504</v>
+        <v>36.384236410409933</v>
       </c>
       <c r="V31">
-        <v>1.883972924968021E-3</v>
+        <v>2.2904598980868379E-3</v>
       </c>
       <c r="W31">
-        <v>-3.5781963579337803E-3</v>
+        <v>-5.0626204592553814E-3</v>
       </c>
       <c r="X31">
-        <v>-5.0136768909181411E-5</v>
+        <v>2.3798721980028683E-4</v>
       </c>
       <c r="Y31">
-        <v>0.25351074069423513</v>
+        <v>0.25226758471922944</v>
       </c>
       <c r="Z31">
-        <v>0.31438042906088132</v>
+        <v>0.3146124714612159</v>
       </c>
       <c r="AA31">
-        <v>5.9667827874250108</v>
+        <v>5.8863744675358847</v>
       </c>
       <c r="AB31">
-        <v>4.9102283394016162E-3</v>
+        <v>4.8557727200676457E-3</v>
       </c>
       <c r="AC31">
-        <v>0.86351572831676959</v>
+        <v>0.8508283929862116</v>
       </c>
     </row>
     <row r="32" spans="1:29">
@@ -3884,257 +3835,174 @@
       <c r="B32" s="8" t="s">
         <v>64</v>
       </c>
+      <c r="C32">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="D32">
+        <v>404</v>
+      </c>
       <c r="E32">
-        <v>2</v>
-      </c>
-      <c r="F32">
-        <v>98.2</v>
+        <v>0.02</v>
+      </c>
+      <c r="F32" s="4">
+        <v>162.93</v>
       </c>
       <c r="G32">
-        <v>1.309214800959835E-2</v>
+        <v>3.0092586846991241E-3</v>
       </c>
       <c r="H32">
-        <v>-3.3001582913460881E-4</v>
+        <v>1.0078628687116636E-3</v>
       </c>
       <c r="I32">
-        <v>3.446120782596767E-2</v>
+        <v>9.9036211019679489E-4</v>
       </c>
       <c r="J32">
-        <v>9.3543411070398132E-4</v>
+        <v>1.061515397678209E-3</v>
       </c>
       <c r="K32">
-        <v>8.7347545773524722E-3</v>
+        <v>1.7758795574271211E-3</v>
       </c>
       <c r="L32">
-        <v>2.1363142359214884E-4</v>
+        <v>3.4714248580651068E-4</v>
       </c>
       <c r="M32">
-        <v>9.837417580758174E-4</v>
+        <v>1.1099932749191073E-3</v>
       </c>
       <c r="N32">
-        <v>-1.218196762588215E-3</v>
+        <v>-1.0136567324002428E-4</v>
       </c>
       <c r="O32">
-        <v>1.1301597764670435E-2</v>
+        <v>1.5016244719135605E-2</v>
       </c>
       <c r="P32">
-        <v>1.2325395052518692E-2</v>
+        <v>3.7799927286455578E-3</v>
       </c>
       <c r="Q32">
-        <v>3.8276226482278318E-2</v>
+        <v>6.4747713087252431E-3</v>
       </c>
       <c r="R32">
-        <v>3.7260431956336935</v>
+        <v>8.8830866728378979</v>
       </c>
       <c r="S32">
-        <v>2.0153723381740587E-4</v>
+        <v>5.1436293795112289E-4</v>
       </c>
       <c r="T32">
-        <v>-6.6150579052835605E-4</v>
+        <v>-9.4550989147549312E-4</v>
       </c>
       <c r="U32">
-        <v>36.384236410409933</v>
+        <v>56.504577538434638</v>
       </c>
       <c r="V32">
-        <v>2.2904598980868379E-3</v>
+        <v>3.5065939590572478E-4</v>
       </c>
       <c r="W32">
-        <v>-5.0626204592553814E-3</v>
+        <v>-7.6061367650050345E-3</v>
       </c>
       <c r="X32">
-        <v>2.3798721980028683E-4</v>
+        <v>3.4587435963442541E-4</v>
       </c>
       <c r="Y32">
-        <v>0.25226758471922944</v>
+        <v>0.32837800504777404</v>
       </c>
       <c r="Z32">
-        <v>0.3146124714612159</v>
+        <v>0.15174506171960808</v>
       </c>
       <c r="AA32">
-        <v>5.8863744675358847</v>
+        <v>5.9022462107645026</v>
       </c>
       <c r="AB32">
-        <v>4.8557727200676457E-3</v>
+        <v>6.4102277084955471E-3</v>
       </c>
       <c r="AC32">
-        <v>0.8508283929862116</v>
+        <v>1.2156469445367131</v>
       </c>
     </row>
     <row r="33" spans="1:29">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33">
-        <v>8.3699999999999992</v>
-      </c>
-      <c r="D33">
-        <v>404</v>
+        <v>64</v>
       </c>
       <c r="E33">
-        <v>0.02</v>
-      </c>
-      <c r="F33" s="4">
-        <v>162.93</v>
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>161.6</v>
       </c>
       <c r="G33">
-        <v>3.0092586846991241E-3</v>
+        <v>4.3646917811188297E-3</v>
       </c>
       <c r="H33">
-        <v>1.0078628687116636E-3</v>
+        <v>1.9789867210923462E-4</v>
       </c>
       <c r="I33">
-        <v>9.9036211019679489E-4</v>
+        <v>1.4261913979779399E-3</v>
       </c>
       <c r="J33">
-        <v>1.061515397678209E-3</v>
+        <v>1.1268351219875378E-3</v>
       </c>
       <c r="K33">
-        <v>1.7758795574271211E-3</v>
+        <v>5.3177977462808982E-3</v>
       </c>
       <c r="L33">
-        <v>3.4714248580651068E-4</v>
+        <v>1.7177320836779045E-4</v>
       </c>
       <c r="M33">
-        <v>1.1099932749191073E-3</v>
+        <v>1.0350123231308592E-3</v>
       </c>
       <c r="N33">
-        <v>-1.0136567324002428E-4</v>
+        <v>1.0977351957800668E-4</v>
       </c>
       <c r="O33">
-        <v>1.5016244719135605E-2</v>
+        <v>1.402667625341549E-2</v>
       </c>
       <c r="P33">
-        <v>3.7799927286455578E-3</v>
+        <v>4.1735775770424402E-3</v>
       </c>
       <c r="Q33">
-        <v>6.4747713087252431E-3</v>
+        <v>6.7411069668097236E-3</v>
       </c>
       <c r="R33">
-        <v>8.8830866728378979</v>
+        <v>8.9782811390961221</v>
       </c>
       <c r="S33">
-        <v>5.1436293795112289E-4</v>
+        <v>4.5463988810596194E-4</v>
       </c>
       <c r="T33">
-        <v>-9.4550989147549312E-4</v>
+        <v>2.236951172311047E-3</v>
       </c>
       <c r="U33">
-        <v>56.504577538434638</v>
+        <v>57.04216373797572</v>
       </c>
       <c r="V33">
-        <v>3.5065939590572478E-4</v>
+        <v>4.131972189433904E-4</v>
       </c>
       <c r="W33">
-        <v>-7.6061367650050345E-3</v>
+        <v>-5.5951773487510799E-3</v>
       </c>
       <c r="X33">
-        <v>3.4587435963442541E-4</v>
+        <v>5.1080940113244332E-4</v>
       </c>
       <c r="Y33">
-        <v>0.32837800504777404</v>
+        <v>0.33426135652727046</v>
       </c>
       <c r="Z33">
-        <v>0.15174506171960808</v>
+        <v>0.16398429631547384</v>
       </c>
       <c r="AA33">
-        <v>5.9022462107645026</v>
+        <v>5.9069352573576213</v>
       </c>
       <c r="AB33">
-        <v>6.4102277084955471E-3</v>
+        <v>6.4314511579873961E-3</v>
       </c>
       <c r="AC33">
-        <v>1.2156469445367131</v>
+        <v>1.2319026100412367</v>
       </c>
     </row>
-    <row r="34" spans="1:29">
-      <c r="A34" t="s">
-        <v>60</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <v>161.6</v>
-      </c>
-      <c r="G34">
-        <v>4.3646917811188297E-3</v>
-      </c>
-      <c r="H34">
-        <v>1.9789867210923462E-4</v>
-      </c>
-      <c r="I34">
-        <v>1.4261913979779399E-3</v>
-      </c>
-      <c r="J34">
-        <v>1.1268351219875378E-3</v>
-      </c>
-      <c r="K34">
-        <v>5.3177977462808982E-3</v>
-      </c>
-      <c r="L34">
-        <v>1.7177320836779045E-4</v>
-      </c>
-      <c r="M34">
-        <v>1.0350123231308592E-3</v>
-      </c>
-      <c r="N34">
-        <v>1.0977351957800668E-4</v>
-      </c>
-      <c r="O34">
-        <v>1.402667625341549E-2</v>
-      </c>
-      <c r="P34">
-        <v>4.1735775770424402E-3</v>
-      </c>
-      <c r="Q34">
-        <v>6.7411069668097236E-3</v>
-      </c>
-      <c r="R34">
-        <v>8.9782811390961221</v>
-      </c>
-      <c r="S34">
-        <v>4.5463988810596194E-4</v>
-      </c>
-      <c r="T34">
-        <v>2.236951172311047E-3</v>
-      </c>
-      <c r="U34">
-        <v>57.04216373797572</v>
-      </c>
-      <c r="V34">
-        <v>4.131972189433904E-4</v>
-      </c>
-      <c r="W34">
-        <v>-5.5951773487510799E-3</v>
-      </c>
-      <c r="X34">
-        <v>5.1080940113244332E-4</v>
-      </c>
-      <c r="Y34">
-        <v>0.33426135652727046</v>
-      </c>
-      <c r="Z34">
-        <v>0.16398429631547384</v>
-      </c>
-      <c r="AA34">
-        <v>5.9069352573576213</v>
-      </c>
-      <c r="AB34">
-        <v>6.4314511579873961E-3</v>
-      </c>
-      <c r="AC34">
-        <v>1.2319026100412367</v>
-      </c>
-    </row>
-    <row r="45" spans="1:29" ht="23">
-      <c r="F45" s="7" t="s">
-        <v>77</v>
+    <row r="44" spans="1:29" ht="23.25">
+      <c r="F44" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>